<commit_message>
Updated version of the model
</commit_message>
<xml_diff>
--- a/v2.0.1/03-Analysis and design/Mappings/Ontology_eForms_Mapping_New Regulation.xlsx
+++ b/v2.0.1/03-Analysis and design/Mappings/Ontology_eForms_Mapping_New Regulation.xlsx
@@ -13936,26 +13936,6 @@
     <t>PIN isA Notice,
 Notice isA Document, 
 Document notifies (subproperty of relatesTo) PlannedProcurementPart,
-PlannedProcurementPart hasAccessTerms AccessTerms,
-AccessTerms hasDownloadURL Channel</t>
-  </si>
-  <si>
-    <t>PIN isA Notice,
-Notice isA Document, 
-Document notifies (subproperty of relatesTo) Procedure,
-Procedure hasAccessTerms AccessTerms,
-AccessTerms hasDownloadURL Channel</t>
-  </si>
-  <si>
-    <t>CN isA Notice,
-Notice isA Document, Document announces (subproperty of relatesTo) Procedure,
-Procedure hasAccessTerms AccessTerms,
-AccessTerms hasDownloadURL Channel</t>
-  </si>
-  <si>
-    <t>PIN isA Notice,
-Notice isA Document, 
-Document notifies (subproperty of relatesTo) PlannedProcurementPart,
 PlannedProcurementPart refersTo Document,
 Document hasOfficalLanguage Code</t>
   </si>
@@ -14009,20 +13989,6 @@
 Notice isA Document, Document announces (subproperty of relatesTo) Procedure,
 Procedure hasAccessTerms AccessTerms,
 AccessTerms hasSomeProcurementDocumentsRestricted Indicator</t>
-  </si>
-  <si>
-    <t>PIN isA Notice,
-Notice isA Document, 
-Document notifies (subproperty of relatesTo) PlannedProcurementPart,
-PlannedProcurementPart hasAccessTerms AccessTerms,
-AccessTerms hasSomeProcurementDocumentsRestrictedJustification Text</t>
-  </si>
-  <si>
-    <t>CN isA Notice,
-Notice isA Document, 
-Document announces (subproperty of relatesTo) PlannedProcurementPart,
-PlannedProcurementPart hasAccessTerms AccessTerms,
-AccessTerms hasSomeProcurementDocumentsRestrictedJustification Tex</t>
   </si>
   <si>
     <t>PIN isA Notice,
@@ -16542,6 +16508,40 @@
 Notice isA Document,
 Document relatesTo Procedure,
 Notice has NotificationContentTypes</t>
+  </si>
+  <si>
+    <t>PIN isA Notice,
+Notice isA Document, 
+Document notifies (subproperty of relatesTo) PlannedProcurementPart,
+PlannedProcurementPart hasAccessTerms AccessTerms,
+AccessTerms hasSomeProcurementDocumentsRestrictedJustification Code</t>
+  </si>
+  <si>
+    <t>CN isA Notice,
+Notice isA Document, 
+Document announces (subproperty of relatesTo) PlannedProcurementPart,
+PlannedProcurementPart hasAccessTerms AccessTerms,
+AccessTerms hasSomeProcurementDocumentsRestrictedJustification Code</t>
+  </si>
+  <si>
+    <t>CN isA Notice,
+Notice isA Document, Document announces (subproperty of relatesTo) Procedure,
+Procedure hasAccessTerms AccessTerms,
+AccessTerms hasProcurementDocumentLandingPage URI</t>
+  </si>
+  <si>
+    <t>PIN isA Notice,
+Notice isA Document, 
+Document notifies (subproperty of relatesTo) Procedure,
+Procedure hasAccessTerms AccessTerms,
+AccessTerms hasProcurementDocumentLandingPage URI</t>
+  </si>
+  <si>
+    <t>PIN isA Notice,
+Notice isA Document, 
+Document notifies (subproperty of relatesTo) PlannedProcurementPart,
+PlannedProcurementPart hasAccessTerms AccessTerms,
+AccessTerms hasProcurementDocumentLandingPage URI</t>
   </si>
 </sst>
 </file>
@@ -17892,6 +17892,15 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="12" fillId="9" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -17902,15 +17911,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18222,6 +18222,15 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -18230,15 +18239,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -18653,8 +18653,8 @@
   <dimension ref="A1:BK312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D185" sqref="D185"/>
+      <pane ySplit="4" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18665,22 +18665,22 @@
     <col min="4" max="4" width="11.1640625" style="85" customWidth="1"/>
     <col min="5" max="5" width="76" style="85" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="85" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" style="85" customWidth="1"/>
-    <col min="8" max="9" width="4.83203125" style="85" customWidth="1"/>
-    <col min="10" max="16" width="4.33203125" style="85" customWidth="1"/>
-    <col min="17" max="17" width="5.1640625" style="85" customWidth="1"/>
-    <col min="18" max="25" width="4.33203125" style="85" customWidth="1"/>
-    <col min="26" max="27" width="4.83203125" style="85" customWidth="1"/>
-    <col min="28" max="28" width="7.6640625" style="85" customWidth="1"/>
-    <col min="29" max="29" width="4.83203125" style="85" customWidth="1"/>
-    <col min="30" max="30" width="4.33203125" style="85" customWidth="1"/>
-    <col min="31" max="31" width="7" style="85" customWidth="1"/>
-    <col min="32" max="32" width="6" style="85" customWidth="1"/>
-    <col min="33" max="33" width="4.33203125" style="85" customWidth="1"/>
-    <col min="34" max="34" width="7.1640625" style="85" customWidth="1"/>
-    <col min="35" max="46" width="4.33203125" style="85" customWidth="1"/>
-    <col min="47" max="47" width="86.1640625" style="85" customWidth="1"/>
-    <col min="48" max="48" width="29" style="85" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="85" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="4.83203125" style="85" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="4.33203125" style="85" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.1640625" style="85" hidden="1" customWidth="1"/>
+    <col min="18" max="25" width="4.33203125" style="85" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="4.83203125" style="85" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="7.6640625" style="85" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="4.83203125" style="85" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="4.33203125" style="85" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="7" style="85" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="6" style="85" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="4.33203125" style="85" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="7.1640625" style="85" hidden="1" customWidth="1"/>
+    <col min="35" max="46" width="4.33203125" style="85" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="86.1640625" style="85" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="29" style="85" hidden="1" customWidth="1"/>
     <col min="49" max="51" width="41.83203125" style="25" customWidth="1"/>
     <col min="52" max="52" width="26.6640625" style="85" customWidth="1"/>
     <col min="53" max="53" width="27.5" style="85" customWidth="1"/>
@@ -18770,11 +18770,11 @@
       <c r="AV1" s="297" t="s">
         <v>267</v>
       </c>
-      <c r="AW1" s="247" t="s">
+      <c r="AW1" s="250" t="s">
         <v>369</v>
       </c>
-      <c r="AX1" s="247"/>
-      <c r="AY1" s="247"/>
+      <c r="AX1" s="250"/>
+      <c r="AY1" s="250"/>
       <c r="AZ1" s="298" t="s">
         <v>266</v>
       </c>
@@ -18933,7 +18933,7 @@
       </c>
       <c r="BA2" s="298"/>
       <c r="BB2" s="299" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC2" s="298" t="s">
         <v>269</v>
@@ -19034,13 +19034,13 @@
       <c r="AT3" s="333"/>
       <c r="AU3" s="43"/>
       <c r="AV3" s="297"/>
-      <c r="AW3" s="247" t="s">
+      <c r="AW3" s="250" t="s">
         <v>370</v>
       </c>
-      <c r="AX3" s="247" t="s">
+      <c r="AX3" s="250" t="s">
         <v>371</v>
       </c>
-      <c r="AY3" s="247" t="s">
+      <c r="AY3" s="250" t="s">
         <v>372</v>
       </c>
       <c r="AZ3" s="298" t="s">
@@ -19199,9 +19199,9 @@
       </c>
       <c r="AU4" s="50"/>
       <c r="AV4" s="297"/>
-      <c r="AW4" s="247"/>
-      <c r="AX4" s="247"/>
-      <c r="AY4" s="247"/>
+      <c r="AW4" s="250"/>
+      <c r="AX4" s="250"/>
+      <c r="AY4" s="250"/>
       <c r="AZ4" s="298"/>
       <c r="BA4" s="298"/>
       <c r="BB4" s="300"/>
@@ -19362,14 +19362,14 @@
       <c r="AX5" s="303"/>
       <c r="AY5" s="303"/>
       <c r="AZ5" s="304" t="s">
-        <v>3207</v>
+        <v>3202</v>
       </c>
       <c r="BA5" s="304"/>
       <c r="BB5" s="182" t="s">
         <v>2064</v>
       </c>
       <c r="BC5" s="304" t="s">
-        <v>3208</v>
+        <v>3203</v>
       </c>
       <c r="BD5" s="304"/>
       <c r="BE5" s="304"/>
@@ -19514,19 +19514,19 @@
       </c>
       <c r="AX6" s="243"/>
       <c r="AY6" s="243"/>
-      <c r="AZ6" s="244" t="s">
-        <v>3190</v>
-      </c>
-      <c r="BA6" s="244"/>
+      <c r="AZ6" s="247" t="s">
+        <v>3185</v>
+      </c>
+      <c r="BA6" s="247"/>
       <c r="BB6" s="179" t="s">
-        <v>3191</v>
-      </c>
-      <c r="BC6" s="244" t="s">
-        <v>3192</v>
-      </c>
-      <c r="BD6" s="244"/>
-      <c r="BE6" s="244"/>
-      <c r="BF6" s="244"/>
+        <v>3186</v>
+      </c>
+      <c r="BC6" s="247" t="s">
+        <v>3187</v>
+      </c>
+      <c r="BD6" s="247"/>
+      <c r="BE6" s="247"/>
+      <c r="BF6" s="247"/>
       <c r="BG6" s="212" t="s">
         <v>2127</v>
       </c>
@@ -19690,7 +19690,7 @@
       </c>
       <c r="BA7" s="234"/>
       <c r="BB7" s="177" t="s">
-        <v>3193</v>
+        <v>3188</v>
       </c>
       <c r="BC7" s="234" t="s">
         <v>2921</v>
@@ -19848,7 +19848,7 @@
         <v>237</v>
       </c>
       <c r="AU8" s="58" t="s">
-        <v>3261</v>
+        <v>3256</v>
       </c>
       <c r="AV8" s="92"/>
       <c r="AW8" s="243" t="s">
@@ -20028,14 +20028,14 @@
       <c r="AX9" s="243"/>
       <c r="AY9" s="243"/>
       <c r="AZ9" s="234" t="s">
-        <v>3194</v>
+        <v>3189</v>
       </c>
       <c r="BA9" s="234"/>
       <c r="BB9" s="177" t="s">
-        <v>3195</v>
+        <v>3190</v>
       </c>
       <c r="BC9" s="234" t="s">
-        <v>3196</v>
+        <v>3191</v>
       </c>
       <c r="BD9" s="234"/>
       <c r="BE9" s="234"/>
@@ -20199,14 +20199,14 @@
       <c r="AX10" s="243"/>
       <c r="AY10" s="243"/>
       <c r="AZ10" s="234" t="s">
-        <v>3197</v>
+        <v>3192</v>
       </c>
       <c r="BA10" s="234"/>
       <c r="BB10" s="177" t="s">
-        <v>3198</v>
+        <v>3193</v>
       </c>
       <c r="BC10" s="234" t="s">
-        <v>3199</v>
+        <v>3194</v>
       </c>
       <c r="BD10" s="234"/>
       <c r="BE10" s="234"/>
@@ -20365,33 +20365,33 @@
         <v>2428</v>
       </c>
       <c r="AW11" s="243" t="s">
-        <v>3462</v>
+        <v>3457</v>
       </c>
       <c r="AX11" s="243"/>
       <c r="AY11" s="243"/>
       <c r="AZ11" s="234" t="s">
-        <v>3463</v>
+        <v>3458</v>
       </c>
       <c r="BA11" s="234"/>
       <c r="BB11" s="177" t="s">
-        <v>3200</v>
+        <v>3195</v>
       </c>
       <c r="BC11" s="234" t="s">
-        <v>3464</v>
+        <v>3459</v>
       </c>
       <c r="BD11" s="234"/>
       <c r="BE11" s="234"/>
       <c r="BF11" s="234"/>
       <c r="BG11" s="136" t="s">
-        <v>3465</v>
+        <v>3460</v>
       </c>
       <c r="BH11" s="236" t="s">
-        <v>3466</v>
+        <v>3461</v>
       </c>
       <c r="BI11" s="237"/>
       <c r="BJ11" s="237"/>
       <c r="BK11" s="201" t="s">
-        <v>3467</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="12" spans="1:63" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -20541,14 +20541,14 @@
       <c r="AX12" s="243"/>
       <c r="AY12" s="243"/>
       <c r="AZ12" s="234" t="s">
-        <v>3201</v>
+        <v>3196</v>
       </c>
       <c r="BA12" s="234"/>
       <c r="BB12" s="177" t="s">
-        <v>3202</v>
+        <v>3197</v>
       </c>
       <c r="BC12" s="234" t="s">
-        <v>3203</v>
+        <v>3198</v>
       </c>
       <c r="BD12" s="234"/>
       <c r="BE12" s="234"/>
@@ -20712,11 +20712,11 @@
       <c r="AX13" s="243"/>
       <c r="AY13" s="243"/>
       <c r="AZ13" s="234" t="s">
-        <v>3204</v>
+        <v>3199</v>
       </c>
       <c r="BA13" s="234"/>
       <c r="BB13" s="177" t="s">
-        <v>3205</v>
+        <v>3200</v>
       </c>
       <c r="BC13" s="234" t="s">
         <v>2915</v>
@@ -22200,7 +22200,7 @@
         <v>2317</v>
       </c>
       <c r="BC22" s="252" t="s">
-        <v>3383</v>
+        <v>3378</v>
       </c>
       <c r="BD22" s="252"/>
       <c r="BE22" s="252"/>
@@ -22369,7 +22369,7 @@
         <v>2293</v>
       </c>
       <c r="BC23" s="252" t="s">
-        <v>3375</v>
+        <v>3370</v>
       </c>
       <c r="BD23" s="252"/>
       <c r="BE23" s="252"/>
@@ -22876,7 +22876,7 @@
         <v>2300</v>
       </c>
       <c r="BC26" s="252" t="s">
-        <v>3376</v>
+        <v>3371</v>
       </c>
       <c r="BD26" s="252"/>
       <c r="BE26" s="252"/>
@@ -23214,7 +23214,7 @@
         <v>2311</v>
       </c>
       <c r="BC28" s="252" t="s">
-        <v>3377</v>
+        <v>3372</v>
       </c>
       <c r="BD28" s="252"/>
       <c r="BE28" s="252"/>
@@ -23385,7 +23385,7 @@
         <v>2326</v>
       </c>
       <c r="BC29" s="252" t="s">
-        <v>3378</v>
+        <v>3373</v>
       </c>
       <c r="BD29" s="252"/>
       <c r="BE29" s="252"/>
@@ -23556,7 +23556,7 @@
         <v>2329</v>
       </c>
       <c r="BC30" s="252" t="s">
-        <v>3379</v>
+        <v>3374</v>
       </c>
       <c r="BD30" s="252"/>
       <c r="BE30" s="252"/>
@@ -23727,7 +23727,7 @@
         <v>2332</v>
       </c>
       <c r="BC31" s="252" t="s">
-        <v>3380</v>
+        <v>3375</v>
       </c>
       <c r="BD31" s="252"/>
       <c r="BE31" s="252"/>
@@ -23898,7 +23898,7 @@
         <v>2335</v>
       </c>
       <c r="BC32" s="252" t="s">
-        <v>3381</v>
+        <v>3376</v>
       </c>
       <c r="BD32" s="252"/>
       <c r="BE32" s="252"/>
@@ -24057,33 +24057,33 @@
         <v>2066</v>
       </c>
       <c r="AW33" s="243" t="s">
-        <v>3456</v>
+        <v>3451</v>
       </c>
       <c r="AX33" s="243"/>
       <c r="AY33" s="243"/>
       <c r="AZ33" s="252" t="s">
-        <v>3456</v>
+        <v>3451</v>
       </c>
       <c r="BA33" s="252"/>
       <c r="BB33" s="177" t="s">
-        <v>3457</v>
+        <v>3452</v>
       </c>
       <c r="BC33" s="252" t="s">
-        <v>3458</v>
+        <v>3453</v>
       </c>
       <c r="BD33" s="252"/>
       <c r="BE33" s="252"/>
       <c r="BF33" s="252"/>
       <c r="BG33" s="136" t="s">
-        <v>3459</v>
+        <v>3454</v>
       </c>
       <c r="BH33" s="236" t="s">
-        <v>3460</v>
+        <v>3455</v>
       </c>
       <c r="BI33" s="237"/>
       <c r="BJ33" s="237"/>
       <c r="BK33" s="201" t="s">
-        <v>3461</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="34" spans="1:63" s="148" customFormat="1" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24238,7 +24238,7 @@
         <v>2338</v>
       </c>
       <c r="BC34" s="252" t="s">
-        <v>3382</v>
+        <v>3377</v>
       </c>
       <c r="BD34" s="252"/>
       <c r="BE34" s="252"/>
@@ -24395,28 +24395,28 @@
       <c r="AU35" s="58"/>
       <c r="AV35" s="102"/>
       <c r="AW35" s="243" t="s">
-        <v>3429</v>
+        <v>3424</v>
       </c>
       <c r="AX35" s="243"/>
       <c r="AY35" s="243"/>
       <c r="AZ35" s="234" t="s">
-        <v>3428</v>
+        <v>3423</v>
       </c>
       <c r="BA35" s="234"/>
       <c r="BB35" s="141" t="s">
         <v>2347</v>
       </c>
       <c r="BC35" s="234" t="s">
-        <v>3427</v>
+        <v>3422</v>
       </c>
       <c r="BD35" s="234"/>
       <c r="BE35" s="234"/>
       <c r="BF35" s="234"/>
       <c r="BG35" s="215" t="s">
-        <v>3426</v>
+        <v>3421</v>
       </c>
       <c r="BH35" s="240" t="s">
-        <v>3425</v>
+        <v>3420</v>
       </c>
       <c r="BI35" s="240"/>
       <c r="BJ35" s="240"/>
@@ -25172,11 +25172,11 @@
       <c r="BC40" s="175" t="s">
         <v>2472</v>
       </c>
-      <c r="BD40" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BE40" s="244"/>
-      <c r="BF40" s="244"/>
+      <c r="BD40" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BE40" s="247"/>
+      <c r="BF40" s="247"/>
       <c r="BG40" s="212" t="s">
         <v>2137</v>
       </c>
@@ -25329,17 +25329,17 @@
       </c>
       <c r="AX41" s="251"/>
       <c r="AY41" s="251"/>
-      <c r="AZ41" s="244" t="s">
+      <c r="AZ41" s="247" t="s">
         <v>2932</v>
       </c>
-      <c r="BA41" s="244"/>
+      <c r="BA41" s="247"/>
       <c r="BB41" s="179" t="s">
         <v>2933</v>
       </c>
-      <c r="BC41" s="244" t="s">
+      <c r="BC41" s="247" t="s">
         <v>2934</v>
       </c>
-      <c r="BD41" s="244"/>
+      <c r="BD41" s="247"/>
       <c r="BE41" s="175" t="s">
         <v>367</v>
       </c>
@@ -25472,17 +25472,17 @@
       </c>
       <c r="AX42" s="251"/>
       <c r="AY42" s="251"/>
-      <c r="AZ42" s="244" t="s">
+      <c r="AZ42" s="247" t="s">
         <v>2935</v>
       </c>
-      <c r="BA42" s="244"/>
+      <c r="BA42" s="247"/>
       <c r="BB42" s="179" t="s">
         <v>2936</v>
       </c>
-      <c r="BC42" s="244" t="s">
+      <c r="BC42" s="247" t="s">
         <v>2937</v>
       </c>
-      <c r="BD42" s="244"/>
+      <c r="BD42" s="247"/>
       <c r="BE42" s="175" t="s">
         <v>367</v>
       </c>
@@ -25686,7 +25686,7 @@
       <c r="AS44" s="67"/>
       <c r="AT44" s="147"/>
       <c r="AU44" s="133" t="s">
-        <v>3385</v>
+        <v>3380</v>
       </c>
       <c r="AV44" s="97"/>
       <c r="AW44" s="243" t="s">
@@ -25694,20 +25694,20 @@
       </c>
       <c r="AX44" s="243"/>
       <c r="AY44" s="243"/>
-      <c r="AZ44" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA44" s="244"/>
-      <c r="BB44" s="244"/>
-      <c r="BC44" s="244"/>
-      <c r="BD44" s="244"/>
-      <c r="BE44" s="244"/>
-      <c r="BF44" s="244"/>
+      <c r="AZ44" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA44" s="247"/>
+      <c r="BB44" s="247"/>
+      <c r="BC44" s="247"/>
+      <c r="BD44" s="247"/>
+      <c r="BE44" s="247"/>
+      <c r="BF44" s="247"/>
       <c r="BG44" s="212" t="s">
-        <v>3396</v>
+        <v>3391</v>
       </c>
       <c r="BH44" s="295" t="s">
-        <v>3386</v>
+        <v>3381</v>
       </c>
       <c r="BI44" s="295"/>
       <c r="BJ44" s="295"/>
@@ -25799,7 +25799,7 @@
       <c r="AS45" s="67"/>
       <c r="AT45" s="147"/>
       <c r="AU45" s="133" t="s">
-        <v>3337</v>
+        <v>3332</v>
       </c>
       <c r="AV45" s="97"/>
       <c r="AW45" s="243" t="s">
@@ -25807,20 +25807,20 @@
       </c>
       <c r="AX45" s="243"/>
       <c r="AY45" s="243"/>
-      <c r="AZ45" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA45" s="244"/>
-      <c r="BB45" s="244"/>
-      <c r="BC45" s="244"/>
-      <c r="BD45" s="244"/>
-      <c r="BE45" s="244"/>
-      <c r="BF45" s="244"/>
+      <c r="AZ45" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA45" s="247"/>
+      <c r="BB45" s="247"/>
+      <c r="BC45" s="247"/>
+      <c r="BD45" s="247"/>
+      <c r="BE45" s="247"/>
+      <c r="BF45" s="247"/>
       <c r="BG45" s="212" t="s">
-        <v>3400</v>
+        <v>3395</v>
       </c>
       <c r="BH45" s="240" t="s">
-        <v>3399</v>
+        <v>3394</v>
       </c>
       <c r="BI45" s="240"/>
       <c r="BJ45" s="240"/>
@@ -25920,20 +25920,20 @@
       </c>
       <c r="AX46" s="243"/>
       <c r="AY46" s="243"/>
-      <c r="AZ46" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA46" s="244"/>
-      <c r="BB46" s="244"/>
-      <c r="BC46" s="244"/>
-      <c r="BD46" s="244"/>
-      <c r="BE46" s="244"/>
-      <c r="BF46" s="244"/>
+      <c r="AZ46" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA46" s="247"/>
+      <c r="BB46" s="247"/>
+      <c r="BC46" s="247"/>
+      <c r="BD46" s="247"/>
+      <c r="BE46" s="247"/>
+      <c r="BF46" s="247"/>
       <c r="BG46" s="212" t="s">
-        <v>3398</v>
+        <v>3393</v>
       </c>
       <c r="BH46" s="240" t="s">
-        <v>3397</v>
+        <v>3392</v>
       </c>
       <c r="BI46" s="240"/>
       <c r="BJ46" s="240"/>
@@ -26757,19 +26757,19 @@
       </c>
       <c r="AX51" s="233"/>
       <c r="AY51" s="233"/>
-      <c r="AZ51" s="244" t="s">
+      <c r="AZ51" s="247" t="s">
         <v>2947</v>
       </c>
-      <c r="BA51" s="244"/>
+      <c r="BA51" s="247"/>
       <c r="BB51" s="179" t="s">
         <v>2948</v>
       </c>
-      <c r="BC51" s="244" t="s">
+      <c r="BC51" s="247" t="s">
         <v>2949</v>
       </c>
-      <c r="BD51" s="244"/>
-      <c r="BE51" s="244"/>
-      <c r="BF51" s="244"/>
+      <c r="BD51" s="247"/>
+      <c r="BE51" s="247"/>
+      <c r="BF51" s="247"/>
       <c r="BG51" s="212" t="s">
         <v>2141</v>
       </c>
@@ -26928,19 +26928,19 @@
       </c>
       <c r="AX52" s="233"/>
       <c r="AY52" s="233"/>
-      <c r="AZ52" s="244" t="s">
+      <c r="AZ52" s="247" t="s">
         <v>2950</v>
       </c>
-      <c r="BA52" s="244"/>
+      <c r="BA52" s="247"/>
       <c r="BB52" s="179" t="s">
         <v>2951</v>
       </c>
-      <c r="BC52" s="244" t="s">
+      <c r="BC52" s="247" t="s">
         <v>2952</v>
       </c>
-      <c r="BD52" s="244"/>
-      <c r="BE52" s="244"/>
-      <c r="BF52" s="244"/>
+      <c r="BD52" s="247"/>
+      <c r="BE52" s="247"/>
+      <c r="BF52" s="247"/>
       <c r="BG52" s="212" t="s">
         <v>2142</v>
       </c>
@@ -27073,18 +27073,18 @@
         <v>2503</v>
       </c>
       <c r="AY53" s="243"/>
-      <c r="AZ53" s="244" t="s">
-        <v>3307</v>
-      </c>
-      <c r="BA53" s="244"/>
+      <c r="AZ53" s="247" t="s">
+        <v>3302</v>
+      </c>
+      <c r="BA53" s="247"/>
       <c r="BB53" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC53" s="244" t="s">
+      <c r="BC53" s="247" t="s">
         <v>2953</v>
       </c>
-      <c r="BD53" s="244"/>
-      <c r="BE53" s="244"/>
+      <c r="BD53" s="247"/>
+      <c r="BE53" s="247"/>
       <c r="BF53" s="175" t="s">
         <v>367</v>
       </c>
@@ -27341,18 +27341,18 @@
         <v>2954</v>
       </c>
       <c r="AY55" s="243"/>
-      <c r="AZ55" s="244" t="s">
-        <v>3212</v>
-      </c>
-      <c r="BA55" s="244"/>
+      <c r="AZ55" s="247" t="s">
+        <v>3207</v>
+      </c>
+      <c r="BA55" s="247"/>
       <c r="BB55" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC55" s="244" t="s">
-        <v>3213</v>
-      </c>
-      <c r="BD55" s="244"/>
-      <c r="BE55" s="244"/>
+      <c r="BC55" s="247" t="s">
+        <v>3208</v>
+      </c>
+      <c r="BD55" s="247"/>
+      <c r="BE55" s="247"/>
       <c r="BF55" s="175" t="s">
         <v>367</v>
       </c>
@@ -27488,18 +27488,18 @@
         <v>2955</v>
       </c>
       <c r="AY56" s="243"/>
-      <c r="AZ56" s="244" t="s">
-        <v>3214</v>
-      </c>
-      <c r="BA56" s="244"/>
+      <c r="AZ56" s="247" t="s">
+        <v>3209</v>
+      </c>
+      <c r="BA56" s="247"/>
       <c r="BB56" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC56" s="244" t="s">
-        <v>3215</v>
-      </c>
-      <c r="BD56" s="244"/>
-      <c r="BE56" s="244"/>
+      <c r="BC56" s="247" t="s">
+        <v>3210</v>
+      </c>
+      <c r="BD56" s="247"/>
+      <c r="BE56" s="247"/>
       <c r="BF56" s="175" t="s">
         <v>367</v>
       </c>
@@ -27820,19 +27820,19 @@
       <c r="AY58" s="251" t="s">
         <v>378</v>
       </c>
-      <c r="AZ58" s="244" t="s">
+      <c r="AZ58" s="247" t="s">
         <v>378</v>
       </c>
-      <c r="BA58" s="244"/>
+      <c r="BA58" s="247"/>
       <c r="BB58" s="179" t="s">
         <v>378</v>
       </c>
-      <c r="BC58" s="244" t="s">
+      <c r="BC58" s="247" t="s">
         <v>378</v>
       </c>
-      <c r="BD58" s="244"/>
-      <c r="BE58" s="244"/>
-      <c r="BF58" s="244"/>
+      <c r="BD58" s="247"/>
+      <c r="BE58" s="247"/>
+      <c r="BF58" s="247"/>
       <c r="BG58" s="216" t="s">
         <v>378</v>
       </c>
@@ -27992,14 +27992,14 @@
       <c r="AX59" s="251"/>
       <c r="AY59" s="251"/>
       <c r="AZ59" s="234" t="s">
-        <v>3216</v>
+        <v>3211</v>
       </c>
       <c r="BA59" s="234"/>
       <c r="BB59" s="177" t="s">
         <v>2956</v>
       </c>
       <c r="BC59" s="234" t="s">
-        <v>3217</v>
+        <v>3212</v>
       </c>
       <c r="BD59" s="234"/>
       <c r="BE59" s="234"/>
@@ -28163,14 +28163,14 @@
       <c r="AX60" s="251"/>
       <c r="AY60" s="251"/>
       <c r="AZ60" s="234" t="s">
-        <v>3218</v>
+        <v>3213</v>
       </c>
       <c r="BA60" s="234"/>
       <c r="BB60" s="177" t="s">
         <v>2957</v>
       </c>
       <c r="BC60" s="234" t="s">
-        <v>3219</v>
+        <v>3214</v>
       </c>
       <c r="BD60" s="234"/>
       <c r="BE60" s="234"/>
@@ -28322,14 +28322,14 @@
         <v>2516</v>
       </c>
       <c r="AZ61" s="234" t="s">
-        <v>3220</v>
+        <v>3215</v>
       </c>
       <c r="BA61" s="234"/>
       <c r="BB61" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC61" s="234" t="s">
-        <v>3221</v>
+        <v>3216</v>
       </c>
       <c r="BD61" s="234"/>
       <c r="BE61" s="234"/>
@@ -28481,14 +28481,14 @@
         <v>2376</v>
       </c>
       <c r="AZ62" s="234" t="s">
-        <v>3222</v>
+        <v>3217</v>
       </c>
       <c r="BA62" s="234"/>
       <c r="BB62" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC62" s="234" t="s">
-        <v>3223</v>
+        <v>3218</v>
       </c>
       <c r="BD62" s="234"/>
       <c r="BE62" s="234"/>
@@ -28632,14 +28632,14 @@
         <v>2522</v>
       </c>
       <c r="AZ63" s="234" t="s">
-        <v>3224</v>
+        <v>3219</v>
       </c>
       <c r="BA63" s="234"/>
       <c r="BB63" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC63" s="234" t="s">
-        <v>3225</v>
+        <v>3220</v>
       </c>
       <c r="BD63" s="234"/>
       <c r="BE63" s="234"/>
@@ -28787,14 +28787,14 @@
         <v>2525</v>
       </c>
       <c r="AZ64" s="234" t="s">
-        <v>3226</v>
+        <v>3221</v>
       </c>
       <c r="BA64" s="234"/>
       <c r="BB64" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC64" s="234" t="s">
-        <v>3227</v>
+        <v>3222</v>
       </c>
       <c r="BD64" s="234"/>
       <c r="BE64" s="234"/>
@@ -28903,19 +28903,19 @@
       </c>
       <c r="AX65" s="243"/>
       <c r="AY65" s="243"/>
-      <c r="AZ65" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA65" s="244"/>
+      <c r="AZ65" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA65" s="247"/>
       <c r="BB65" s="179" t="s">
         <v>2958</v>
       </c>
-      <c r="BC65" s="244" t="s">
-        <v>3228</v>
-      </c>
-      <c r="BD65" s="244"/>
-      <c r="BE65" s="244"/>
-      <c r="BF65" s="244"/>
+      <c r="BC65" s="247" t="s">
+        <v>3223</v>
+      </c>
+      <c r="BD65" s="247"/>
+      <c r="BE65" s="247"/>
+      <c r="BF65" s="247"/>
       <c r="BG65" s="216" t="s">
         <v>367</v>
       </c>
@@ -29016,19 +29016,19 @@
       </c>
       <c r="AX66" s="243"/>
       <c r="AY66" s="243"/>
-      <c r="AZ66" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA66" s="244"/>
+      <c r="AZ66" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA66" s="247"/>
       <c r="BB66" s="179" t="s">
         <v>2959</v>
       </c>
-      <c r="BC66" s="244" t="s">
-        <v>3229</v>
-      </c>
-      <c r="BD66" s="244"/>
-      <c r="BE66" s="244"/>
-      <c r="BF66" s="244"/>
+      <c r="BC66" s="247" t="s">
+        <v>3224</v>
+      </c>
+      <c r="BD66" s="247"/>
+      <c r="BE66" s="247"/>
+      <c r="BF66" s="247"/>
       <c r="BG66" s="216" t="s">
         <v>367</v>
       </c>
@@ -29339,11 +29339,11 @@
       <c r="AV68" s="91" t="s">
         <v>2530</v>
       </c>
-      <c r="AW68" s="246" t="s">
+      <c r="AW68" s="249" t="s">
         <v>2960</v>
       </c>
-      <c r="AX68" s="246"/>
-      <c r="AY68" s="246"/>
+      <c r="AX68" s="249"/>
+      <c r="AY68" s="249"/>
       <c r="AZ68" s="234" t="s">
         <v>2961</v>
       </c>
@@ -29510,11 +29510,11 @@
       <c r="AV69" s="91" t="s">
         <v>2531</v>
       </c>
-      <c r="AW69" s="246" t="s">
+      <c r="AW69" s="249" t="s">
         <v>2964</v>
       </c>
-      <c r="AX69" s="246"/>
-      <c r="AY69" s="246"/>
+      <c r="AX69" s="249"/>
+      <c r="AY69" s="249"/>
       <c r="AZ69" s="234" t="s">
         <v>2965</v>
       </c>
@@ -29681,11 +29681,11 @@
       <c r="AV70" s="91" t="s">
         <v>2532</v>
       </c>
-      <c r="AW70" s="246" t="s">
+      <c r="AW70" s="249" t="s">
         <v>2968</v>
       </c>
-      <c r="AX70" s="246"/>
-      <c r="AY70" s="246"/>
+      <c r="AX70" s="249"/>
+      <c r="AY70" s="249"/>
       <c r="AZ70" s="234" t="s">
         <v>2969</v>
       </c>
@@ -29852,11 +29852,11 @@
       <c r="AV71" s="91" t="s">
         <v>2533</v>
       </c>
-      <c r="AW71" s="246" t="s">
+      <c r="AW71" s="249" t="s">
         <v>2972</v>
       </c>
-      <c r="AX71" s="246"/>
-      <c r="AY71" s="246"/>
+      <c r="AX71" s="249"/>
+      <c r="AY71" s="249"/>
       <c r="AZ71" s="234" t="s">
         <v>2973</v>
       </c>
@@ -30023,11 +30023,11 @@
       <c r="AV72" s="91" t="s">
         <v>2534</v>
       </c>
-      <c r="AW72" s="246" t="s">
+      <c r="AW72" s="249" t="s">
         <v>2976</v>
       </c>
-      <c r="AX72" s="246"/>
-      <c r="AY72" s="246"/>
+      <c r="AX72" s="249"/>
+      <c r="AY72" s="249"/>
       <c r="AZ72" s="234" t="s">
         <v>2977</v>
       </c>
@@ -30194,11 +30194,11 @@
       <c r="AV73" s="97" t="s">
         <v>2536</v>
       </c>
-      <c r="AW73" s="246" t="s">
+      <c r="AW73" s="249" t="s">
         <v>2980</v>
       </c>
-      <c r="AX73" s="246"/>
-      <c r="AY73" s="246"/>
+      <c r="AX73" s="249"/>
+      <c r="AY73" s="249"/>
       <c r="AZ73" s="234" t="s">
         <v>2981</v>
       </c>
@@ -30365,11 +30365,11 @@
       <c r="AV74" s="96" t="s">
         <v>2538</v>
       </c>
-      <c r="AW74" s="246" t="s">
+      <c r="AW74" s="249" t="s">
         <v>2984</v>
       </c>
-      <c r="AX74" s="246"/>
-      <c r="AY74" s="246"/>
+      <c r="AX74" s="249"/>
+      <c r="AY74" s="249"/>
       <c r="AZ74" s="234" t="s">
         <v>2985</v>
       </c>
@@ -31010,18 +31010,18 @@
       </c>
       <c r="AX78" s="243"/>
       <c r="AY78" s="243"/>
-      <c r="AZ78" s="244" t="s">
+      <c r="AZ78" s="247" t="s">
         <v>2997</v>
       </c>
-      <c r="BA78" s="244"/>
+      <c r="BA78" s="247"/>
       <c r="BB78" s="179" t="s">
         <v>2998</v>
       </c>
-      <c r="BC78" s="244" t="s">
+      <c r="BC78" s="247" t="s">
         <v>2999</v>
       </c>
-      <c r="BD78" s="244"/>
-      <c r="BE78" s="244"/>
+      <c r="BD78" s="247"/>
+      <c r="BE78" s="247"/>
       <c r="BF78" s="175" t="s">
         <v>367</v>
       </c>
@@ -31177,18 +31177,18 @@
       </c>
       <c r="AX79" s="243"/>
       <c r="AY79" s="243"/>
-      <c r="AZ79" s="244" t="s">
+      <c r="AZ79" s="247" t="s">
         <v>3001</v>
       </c>
-      <c r="BA79" s="244"/>
+      <c r="BA79" s="247"/>
       <c r="BB79" s="179" t="s">
         <v>3002</v>
       </c>
-      <c r="BC79" s="244" t="s">
+      <c r="BC79" s="247" t="s">
         <v>3003</v>
       </c>
-      <c r="BD79" s="244"/>
-      <c r="BE79" s="244"/>
+      <c r="BD79" s="247"/>
+      <c r="BE79" s="247"/>
       <c r="BF79" s="175" t="s">
         <v>367</v>
       </c>
@@ -31795,19 +31795,19 @@
       <c r="AY83" s="178" t="s">
         <v>3012</v>
       </c>
-      <c r="AZ83" s="244" t="s">
+      <c r="AZ83" s="247" t="s">
         <v>3013</v>
       </c>
-      <c r="BA83" s="244"/>
+      <c r="BA83" s="247"/>
       <c r="BB83" s="179" t="s">
         <v>3014</v>
       </c>
-      <c r="BC83" s="244" t="s">
+      <c r="BC83" s="247" t="s">
         <v>3015</v>
       </c>
-      <c r="BD83" s="244"/>
-      <c r="BE83" s="244"/>
-      <c r="BF83" s="244"/>
+      <c r="BD83" s="247"/>
+      <c r="BE83" s="247"/>
+      <c r="BF83" s="247"/>
       <c r="BG83" s="212" t="s">
         <v>2158</v>
       </c>
@@ -32224,19 +32224,19 @@
       <c r="AY86" s="142" t="s">
         <v>3016</v>
       </c>
-      <c r="AZ86" s="244" t="s">
-        <v>3209</v>
-      </c>
-      <c r="BA86" s="244"/>
+      <c r="AZ86" s="247" t="s">
+        <v>3204</v>
+      </c>
+      <c r="BA86" s="247"/>
       <c r="BB86" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC86" s="244" t="s">
+      <c r="BC86" s="247" t="s">
         <v>3017</v>
       </c>
-      <c r="BD86" s="244"/>
-      <c r="BE86" s="244"/>
-      <c r="BF86" s="244"/>
+      <c r="BD86" s="247"/>
+      <c r="BE86" s="247"/>
+      <c r="BF86" s="247"/>
       <c r="BG86" s="212" t="s">
         <v>2160</v>
       </c>
@@ -32365,21 +32365,21 @@
       </c>
       <c r="AX87" s="243"/>
       <c r="AY87" s="142" t="s">
-        <v>3231</v>
-      </c>
-      <c r="AZ87" s="244" t="s">
-        <v>3230</v>
-      </c>
-      <c r="BA87" s="244"/>
+        <v>3226</v>
+      </c>
+      <c r="AZ87" s="247" t="s">
+        <v>3225</v>
+      </c>
+      <c r="BA87" s="247"/>
       <c r="BB87" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC87" s="244" t="s">
+      <c r="BC87" s="247" t="s">
         <v>3018</v>
       </c>
-      <c r="BD87" s="244"/>
-      <c r="BE87" s="244"/>
-      <c r="BF87" s="244"/>
+      <c r="BD87" s="247"/>
+      <c r="BE87" s="247"/>
+      <c r="BF87" s="247"/>
       <c r="BG87" s="216" t="s">
         <v>367</v>
       </c>
@@ -32470,21 +32470,21 @@
       </c>
       <c r="AX88" s="243"/>
       <c r="AY88" s="243"/>
-      <c r="AZ88" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA88" s="244"/>
+      <c r="AZ88" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA88" s="247"/>
       <c r="BB88" s="179" t="s">
         <v>367</v>
       </c>
       <c r="BC88" s="175" t="s">
         <v>3019</v>
       </c>
-      <c r="BD88" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BE88" s="244"/>
-      <c r="BF88" s="244"/>
+      <c r="BD88" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BE88" s="247"/>
+      <c r="BF88" s="247"/>
       <c r="BG88" s="216" t="s">
         <v>367</v>
       </c>
@@ -32577,21 +32577,21 @@
       </c>
       <c r="AX89" s="243"/>
       <c r="AY89" s="243"/>
-      <c r="AZ89" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA89" s="244"/>
+      <c r="AZ89" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA89" s="247"/>
       <c r="BB89" s="179" t="s">
         <v>367</v>
       </c>
       <c r="BC89" s="175" t="s">
         <v>3020</v>
       </c>
-      <c r="BD89" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BE89" s="244"/>
-      <c r="BF89" s="244"/>
+      <c r="BD89" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BE89" s="247"/>
+      <c r="BF89" s="247"/>
       <c r="BG89" s="216" t="s">
         <v>367</v>
       </c>
@@ -32694,15 +32694,15 @@
       </c>
       <c r="AX90" s="243"/>
       <c r="AY90" s="243"/>
-      <c r="AZ90" s="245" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA90" s="245"/>
-      <c r="BB90" s="245"/>
-      <c r="BC90" s="245"/>
-      <c r="BD90" s="245"/>
-      <c r="BE90" s="245"/>
-      <c r="BF90" s="245"/>
+      <c r="AZ90" s="248" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA90" s="248"/>
+      <c r="BB90" s="248"/>
+      <c r="BC90" s="248"/>
+      <c r="BD90" s="248"/>
+      <c r="BE90" s="248"/>
+      <c r="BF90" s="248"/>
       <c r="BG90" s="217" t="s">
         <v>2161</v>
       </c>
@@ -32805,15 +32805,15 @@
       </c>
       <c r="AX91" s="243"/>
       <c r="AY91" s="243"/>
-      <c r="AZ91" s="245" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA91" s="245"/>
-      <c r="BB91" s="245"/>
-      <c r="BC91" s="245"/>
-      <c r="BD91" s="245"/>
-      <c r="BE91" s="245"/>
-      <c r="BF91" s="245"/>
+      <c r="AZ91" s="248" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA91" s="248"/>
+      <c r="BB91" s="248"/>
+      <c r="BC91" s="248"/>
+      <c r="BD91" s="248"/>
+      <c r="BE91" s="248"/>
+      <c r="BF91" s="248"/>
       <c r="BG91" s="217" t="s">
         <v>2162</v>
       </c>
@@ -32916,15 +32916,15 @@
       </c>
       <c r="AX92" s="243"/>
       <c r="AY92" s="243"/>
-      <c r="AZ92" s="245" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA92" s="245"/>
-      <c r="BB92" s="245"/>
-      <c r="BC92" s="245"/>
-      <c r="BD92" s="245"/>
-      <c r="BE92" s="245"/>
-      <c r="BF92" s="245"/>
+      <c r="AZ92" s="248" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA92" s="248"/>
+      <c r="BB92" s="248"/>
+      <c r="BC92" s="248"/>
+      <c r="BD92" s="248"/>
+      <c r="BE92" s="248"/>
+      <c r="BF92" s="248"/>
       <c r="BG92" s="217" t="s">
         <v>2163</v>
       </c>
@@ -33041,19 +33041,19 @@
       <c r="AY93" s="142" t="s">
         <v>3021</v>
       </c>
-      <c r="AZ93" s="244" t="s">
+      <c r="AZ93" s="247" t="s">
         <v>3022</v>
       </c>
-      <c r="BA93" s="244"/>
+      <c r="BA93" s="247"/>
       <c r="BB93" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC93" s="244" t="s">
+      <c r="BC93" s="247" t="s">
         <v>3023</v>
       </c>
-      <c r="BD93" s="244"/>
-      <c r="BE93" s="244"/>
-      <c r="BF93" s="244"/>
+      <c r="BD93" s="247"/>
+      <c r="BE93" s="247"/>
+      <c r="BF93" s="247"/>
       <c r="BG93" s="216" t="s">
         <v>367</v>
       </c>
@@ -33168,19 +33168,19 @@
       <c r="AY94" s="142" t="s">
         <v>3024</v>
       </c>
-      <c r="AZ94" s="244" t="s">
+      <c r="AZ94" s="247" t="s">
         <v>3025</v>
       </c>
-      <c r="BA94" s="244"/>
+      <c r="BA94" s="247"/>
       <c r="BB94" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC94" s="244" t="s">
+      <c r="BC94" s="247" t="s">
         <v>3026</v>
       </c>
-      <c r="BD94" s="244"/>
-      <c r="BE94" s="244"/>
-      <c r="BF94" s="244"/>
+      <c r="BD94" s="247"/>
+      <c r="BE94" s="247"/>
+      <c r="BF94" s="247"/>
       <c r="BG94" s="216" t="s">
         <v>367</v>
       </c>
@@ -33295,19 +33295,19 @@
       <c r="AY95" s="142" t="s">
         <v>3027</v>
       </c>
-      <c r="AZ95" s="244" t="s">
+      <c r="AZ95" s="247" t="s">
         <v>3028</v>
       </c>
-      <c r="BA95" s="244"/>
+      <c r="BA95" s="247"/>
       <c r="BB95" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC95" s="244" t="s">
+      <c r="BC95" s="247" t="s">
         <v>3029</v>
       </c>
-      <c r="BD95" s="244"/>
-      <c r="BE95" s="244"/>
-      <c r="BF95" s="244"/>
+      <c r="BD95" s="247"/>
+      <c r="BE95" s="247"/>
+      <c r="BF95" s="247"/>
       <c r="BG95" s="216" t="s">
         <v>367</v>
       </c>
@@ -33530,19 +33530,19 @@
       <c r="AY97" s="142" t="s">
         <v>3030</v>
       </c>
-      <c r="AZ97" s="244" t="s">
+      <c r="AZ97" s="247" t="s">
         <v>3031</v>
       </c>
-      <c r="BA97" s="244"/>
+      <c r="BA97" s="247"/>
       <c r="BB97" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC97" s="244" t="s">
+      <c r="BC97" s="247" t="s">
         <v>3032</v>
       </c>
-      <c r="BD97" s="244"/>
-      <c r="BE97" s="244"/>
-      <c r="BF97" s="244"/>
+      <c r="BD97" s="247"/>
+      <c r="BE97" s="247"/>
+      <c r="BF97" s="247"/>
       <c r="BG97" s="216" t="s">
         <v>367</v>
       </c>
@@ -33657,19 +33657,19 @@
       <c r="AY98" s="142" t="s">
         <v>3033</v>
       </c>
-      <c r="AZ98" s="244" t="s">
+      <c r="AZ98" s="247" t="s">
         <v>3033</v>
       </c>
-      <c r="BA98" s="244"/>
+      <c r="BA98" s="247"/>
       <c r="BB98" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC98" s="244" t="s">
+      <c r="BC98" s="247" t="s">
         <v>3034</v>
       </c>
-      <c r="BD98" s="244"/>
-      <c r="BE98" s="244"/>
-      <c r="BF98" s="244"/>
+      <c r="BD98" s="247"/>
+      <c r="BE98" s="247"/>
+      <c r="BF98" s="247"/>
       <c r="BG98" s="216" t="s">
         <v>367</v>
       </c>
@@ -33891,19 +33891,19 @@
       <c r="AY100" s="142" t="s">
         <v>3035</v>
       </c>
-      <c r="AZ100" s="244" t="s">
+      <c r="AZ100" s="247" t="s">
         <v>3035</v>
       </c>
-      <c r="BA100" s="244"/>
+      <c r="BA100" s="247"/>
       <c r="BB100" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC100" s="244" t="s">
+      <c r="BC100" s="247" t="s">
         <v>3036</v>
       </c>
-      <c r="BD100" s="244"/>
-      <c r="BE100" s="244"/>
-      <c r="BF100" s="244"/>
+      <c r="BD100" s="247"/>
+      <c r="BE100" s="247"/>
+      <c r="BF100" s="247"/>
       <c r="BG100" s="216" t="s">
         <v>367</v>
       </c>
@@ -34014,19 +34014,19 @@
       <c r="AY101" s="142" t="s">
         <v>3037</v>
       </c>
-      <c r="AZ101" s="244" t="s">
+      <c r="AZ101" s="247" t="s">
         <v>3037</v>
       </c>
-      <c r="BA101" s="244"/>
+      <c r="BA101" s="247"/>
       <c r="BB101" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC101" s="244" t="s">
+      <c r="BC101" s="247" t="s">
         <v>3038</v>
       </c>
-      <c r="BD101" s="244"/>
-      <c r="BE101" s="244"/>
-      <c r="BF101" s="244"/>
+      <c r="BD101" s="247"/>
+      <c r="BE101" s="247"/>
+      <c r="BF101" s="247"/>
       <c r="BG101" s="216" t="s">
         <v>367</v>
       </c>
@@ -34139,19 +34139,19 @@
       <c r="AY102" s="142" t="s">
         <v>3039</v>
       </c>
-      <c r="AZ102" s="244" t="s">
+      <c r="AZ102" s="247" t="s">
         <v>3040</v>
       </c>
-      <c r="BA102" s="244"/>
+      <c r="BA102" s="247"/>
       <c r="BB102" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC102" s="244" t="s">
+      <c r="BC102" s="247" t="s">
         <v>3041</v>
       </c>
-      <c r="BD102" s="244"/>
-      <c r="BE102" s="244"/>
-      <c r="BF102" s="244"/>
+      <c r="BD102" s="247"/>
+      <c r="BE102" s="247"/>
+      <c r="BF102" s="247"/>
       <c r="BG102" s="216" t="s">
         <v>367</v>
       </c>
@@ -34264,19 +34264,19 @@
       <c r="AY103" s="142" t="s">
         <v>3042</v>
       </c>
-      <c r="AZ103" s="244" t="s">
+      <c r="AZ103" s="247" t="s">
         <v>3043</v>
       </c>
-      <c r="BA103" s="244"/>
+      <c r="BA103" s="247"/>
       <c r="BB103" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC103" s="244" t="s">
+      <c r="BC103" s="247" t="s">
         <v>3044</v>
       </c>
-      <c r="BD103" s="244"/>
-      <c r="BE103" s="244"/>
-      <c r="BF103" s="244"/>
+      <c r="BD103" s="247"/>
+      <c r="BE103" s="247"/>
+      <c r="BF103" s="247"/>
       <c r="BG103" s="216" t="s">
         <v>367</v>
       </c>
@@ -34359,21 +34359,21 @@
       </c>
       <c r="AX104" s="243"/>
       <c r="AY104" s="243"/>
-      <c r="AZ104" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA104" s="244"/>
+      <c r="AZ104" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA104" s="247"/>
       <c r="BB104" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC104" s="244" t="s">
+      <c r="BC104" s="247" t="s">
         <v>3045</v>
       </c>
-      <c r="BD104" s="244"/>
-      <c r="BE104" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BF104" s="244"/>
+      <c r="BD104" s="247"/>
+      <c r="BE104" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BF104" s="247"/>
       <c r="BG104" s="216" t="s">
         <v>367</v>
       </c>
@@ -34614,18 +34614,18 @@
       </c>
       <c r="AX107" s="243"/>
       <c r="AY107" s="243"/>
-      <c r="AZ107" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA107" s="244"/>
+      <c r="AZ107" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA107" s="247"/>
       <c r="BB107" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC107" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD107" s="244"/>
-      <c r="BE107" s="244"/>
+      <c r="BC107" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD107" s="247"/>
+      <c r="BE107" s="247"/>
       <c r="BF107" s="175" t="s">
         <v>3046</v>
       </c>
@@ -34711,18 +34711,18 @@
       </c>
       <c r="AX108" s="243"/>
       <c r="AY108" s="243"/>
-      <c r="AZ108" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA108" s="244"/>
+      <c r="AZ108" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA108" s="247"/>
       <c r="BB108" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC108" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD108" s="244"/>
-      <c r="BE108" s="244"/>
+      <c r="BC108" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD108" s="247"/>
+      <c r="BE108" s="247"/>
       <c r="BF108" s="175" t="s">
         <v>3047</v>
       </c>
@@ -34808,18 +34808,18 @@
       </c>
       <c r="AX109" s="243"/>
       <c r="AY109" s="243"/>
-      <c r="AZ109" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA109" s="244"/>
+      <c r="AZ109" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA109" s="247"/>
       <c r="BB109" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC109" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD109" s="244"/>
-      <c r="BE109" s="244"/>
+      <c r="BC109" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD109" s="247"/>
+      <c r="BE109" s="247"/>
       <c r="BF109" s="175" t="s">
         <v>3048</v>
       </c>
@@ -34905,18 +34905,18 @@
       </c>
       <c r="AX110" s="243"/>
       <c r="AY110" s="243"/>
-      <c r="AZ110" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA110" s="244"/>
+      <c r="AZ110" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA110" s="247"/>
       <c r="BB110" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC110" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD110" s="244"/>
-      <c r="BE110" s="244"/>
+      <c r="BC110" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD110" s="247"/>
+      <c r="BE110" s="247"/>
       <c r="BF110" s="175" t="s">
         <v>3049</v>
       </c>
@@ -35002,18 +35002,18 @@
       </c>
       <c r="AX111" s="243"/>
       <c r="AY111" s="243"/>
-      <c r="AZ111" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA111" s="244"/>
+      <c r="AZ111" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA111" s="247"/>
       <c r="BB111" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC111" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD111" s="244"/>
-      <c r="BE111" s="244"/>
+      <c r="BC111" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD111" s="247"/>
+      <c r="BE111" s="247"/>
       <c r="BF111" s="175" t="s">
         <v>3050</v>
       </c>
@@ -35099,18 +35099,18 @@
       </c>
       <c r="AX112" s="243"/>
       <c r="AY112" s="243"/>
-      <c r="AZ112" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA112" s="244"/>
+      <c r="AZ112" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA112" s="247"/>
       <c r="BB112" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC112" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD112" s="244"/>
-      <c r="BE112" s="244"/>
+      <c r="BC112" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD112" s="247"/>
+      <c r="BE112" s="247"/>
       <c r="BF112" s="175" t="s">
         <v>3051</v>
       </c>
@@ -35196,18 +35196,18 @@
       </c>
       <c r="AX113" s="243"/>
       <c r="AY113" s="243"/>
-      <c r="AZ113" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA113" s="244"/>
+      <c r="AZ113" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BA113" s="247"/>
       <c r="BB113" s="179" t="s">
         <v>367</v>
       </c>
-      <c r="BC113" s="244" t="s">
-        <v>367</v>
-      </c>
-      <c r="BD113" s="244"/>
-      <c r="BE113" s="244"/>
+      <c r="BC113" s="247" t="s">
+        <v>367</v>
+      </c>
+      <c r="BD113" s="247"/>
+      <c r="BE113" s="247"/>
       <c r="BF113" s="175" t="s">
         <v>3052</v>
       </c>
@@ -35428,7 +35428,7 @@
       <c r="AS115" s="67"/>
       <c r="AT115" s="147"/>
       <c r="AU115" s="133" t="s">
-        <v>3269</v>
+        <v>3264</v>
       </c>
       <c r="AV115" s="97"/>
       <c r="AW115" s="243" t="s">
@@ -35436,17 +35436,17 @@
       </c>
       <c r="AX115" s="243"/>
       <c r="AY115" s="142" t="s">
-        <v>3293</v>
+        <v>3288</v>
       </c>
       <c r="AZ115" s="234" t="s">
-        <v>3293</v>
+        <v>3288</v>
       </c>
       <c r="BA115" s="234"/>
       <c r="BB115" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC115" s="234" t="s">
-        <v>3294</v>
+        <v>3289</v>
       </c>
       <c r="BD115" s="234"/>
       <c r="BE115" s="234"/>
@@ -35668,7 +35668,7 @@
       <c r="AS117" s="67"/>
       <c r="AT117" s="147"/>
       <c r="AU117" s="133" t="s">
-        <v>3270</v>
+        <v>3265</v>
       </c>
       <c r="AV117" s="97"/>
       <c r="AW117" s="243" t="s">
@@ -35676,17 +35676,17 @@
       </c>
       <c r="AX117" s="243"/>
       <c r="AY117" s="223" t="s">
-        <v>3237</v>
+        <v>3232</v>
       </c>
       <c r="AZ117" s="234" t="s">
-        <v>3237</v>
+        <v>3232</v>
       </c>
       <c r="BA117" s="234"/>
       <c r="BB117" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC117" s="234" t="s">
-        <v>3238</v>
+        <v>3233</v>
       </c>
       <c r="BD117" s="234"/>
       <c r="BE117" s="234"/>
@@ -35797,7 +35797,7 @@
       <c r="AS118" s="67"/>
       <c r="AT118" s="147"/>
       <c r="AU118" s="133" t="s">
-        <v>3313</v>
+        <v>3308</v>
       </c>
       <c r="AV118" s="97"/>
       <c r="AW118" s="243" t="s">
@@ -35805,17 +35805,17 @@
       </c>
       <c r="AX118" s="243"/>
       <c r="AY118" s="223" t="s">
-        <v>3453</v>
+        <v>3448</v>
       </c>
       <c r="AZ118" s="238" t="s">
-        <v>3454</v>
+        <v>3449</v>
       </c>
       <c r="BA118" s="238"/>
       <c r="BB118" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC118" s="238" t="s">
-        <v>3455</v>
+        <v>3450</v>
       </c>
       <c r="BD118" s="238"/>
       <c r="BE118" s="238"/>
@@ -35932,17 +35932,17 @@
       </c>
       <c r="AX119" s="243"/>
       <c r="AY119" s="224" t="s">
-        <v>3295</v>
+        <v>3290</v>
       </c>
       <c r="AZ119" s="234" t="s">
-        <v>3295</v>
+        <v>3290</v>
       </c>
       <c r="BA119" s="234"/>
       <c r="BB119" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC119" s="234" t="s">
-        <v>3296</v>
+        <v>3291</v>
       </c>
       <c r="BD119" s="234"/>
       <c r="BE119" s="234"/>
@@ -36059,17 +36059,17 @@
       </c>
       <c r="AX120" s="243"/>
       <c r="AY120" s="224" t="s">
-        <v>3297</v>
+        <v>3292</v>
       </c>
       <c r="AZ120" s="234" t="s">
-        <v>3297</v>
+        <v>3292</v>
       </c>
       <c r="BA120" s="234"/>
       <c r="BB120" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC120" s="234" t="s">
-        <v>3298</v>
+        <v>3293</v>
       </c>
       <c r="BD120" s="234"/>
       <c r="BE120" s="234"/>
@@ -36095,7 +36095,7 @@
         <v>2629</v>
       </c>
       <c r="D121" s="227" t="s">
-        <v>3315</v>
+        <v>3310</v>
       </c>
       <c r="E121" s="54" t="s">
         <v>1984</v>
@@ -36176,7 +36176,7 @@
       <c r="AS121" s="67"/>
       <c r="AT121" s="147"/>
       <c r="AU121" s="133" t="s">
-        <v>3314</v>
+        <v>3309</v>
       </c>
       <c r="AV121" s="97"/>
       <c r="AW121" s="243" t="s">
@@ -36184,21 +36184,21 @@
       </c>
       <c r="AX121" s="243"/>
       <c r="AY121" s="224" t="s">
-        <v>3260</v>
-      </c>
-      <c r="AZ121" s="248" t="s">
-        <v>3260</v>
-      </c>
-      <c r="BA121" s="249"/>
+        <v>3255</v>
+      </c>
+      <c r="AZ121" s="244" t="s">
+        <v>3255</v>
+      </c>
+      <c r="BA121" s="246"/>
       <c r="BB121" s="177" t="s">
-        <v>3243</v>
-      </c>
-      <c r="BC121" s="248" t="s">
-        <v>3299</v>
-      </c>
-      <c r="BD121" s="250"/>
-      <c r="BE121" s="250"/>
-      <c r="BF121" s="249"/>
+        <v>3238</v>
+      </c>
+      <c r="BC121" s="244" t="s">
+        <v>3294</v>
+      </c>
+      <c r="BD121" s="245"/>
+      <c r="BE121" s="245"/>
+      <c r="BF121" s="246"/>
       <c r="BG121" s="214" t="s">
         <v>367</v>
       </c>
@@ -36220,7 +36220,7 @@
         <v>2630</v>
       </c>
       <c r="D122" s="228" t="s">
-        <v>3316</v>
+        <v>3311</v>
       </c>
       <c r="E122" s="51" t="s">
         <v>1985</v>
@@ -36326,7 +36326,7 @@
         <v>2631</v>
       </c>
       <c r="D123" s="227" t="s">
-        <v>3316</v>
+        <v>3311</v>
       </c>
       <c r="E123" s="54" t="s">
         <v>1986</v>
@@ -36407,7 +36407,7 @@
       <c r="AS123" s="67"/>
       <c r="AT123" s="147"/>
       <c r="AU123" s="280" t="s">
-        <v>3332</v>
+        <v>3327</v>
       </c>
       <c r="AV123" s="97"/>
       <c r="AW123" s="243" t="s">
@@ -36415,21 +36415,21 @@
       </c>
       <c r="AX123" s="243"/>
       <c r="AY123" s="226" t="s">
-        <v>3302</v>
-      </c>
-      <c r="AZ123" s="248" t="s">
-        <v>3301</v>
-      </c>
-      <c r="BA123" s="249"/>
+        <v>3297</v>
+      </c>
+      <c r="AZ123" s="244" t="s">
+        <v>3296</v>
+      </c>
+      <c r="BA123" s="246"/>
       <c r="BB123" s="177" t="s">
-        <v>3243</v>
-      </c>
-      <c r="BC123" s="248" t="s">
-        <v>3300</v>
-      </c>
-      <c r="BD123" s="250"/>
-      <c r="BE123" s="250"/>
-      <c r="BF123" s="249"/>
+        <v>3238</v>
+      </c>
+      <c r="BC123" s="244" t="s">
+        <v>3295</v>
+      </c>
+      <c r="BD123" s="245"/>
+      <c r="BE123" s="245"/>
+      <c r="BF123" s="246"/>
       <c r="BG123" s="214" t="s">
         <v>367</v>
       </c>
@@ -36451,7 +36451,7 @@
         <v>1879</v>
       </c>
       <c r="D124" s="227" t="s">
-        <v>3318</v>
+        <v>3313</v>
       </c>
       <c r="E124" s="54" t="s">
         <v>1987</v>
@@ -36538,21 +36538,21 @@
       </c>
       <c r="AX124" s="243"/>
       <c r="AY124" s="226" t="s">
-        <v>3303</v>
-      </c>
-      <c r="AZ124" s="248" t="s">
-        <v>3303</v>
-      </c>
-      <c r="BA124" s="249"/>
+        <v>3298</v>
+      </c>
+      <c r="AZ124" s="244" t="s">
+        <v>3298</v>
+      </c>
+      <c r="BA124" s="246"/>
       <c r="BB124" s="177" t="s">
-        <v>3243</v>
-      </c>
-      <c r="BC124" s="248" t="s">
-        <v>3304</v>
-      </c>
-      <c r="BD124" s="250"/>
-      <c r="BE124" s="250"/>
-      <c r="BF124" s="249"/>
+        <v>3238</v>
+      </c>
+      <c r="BC124" s="244" t="s">
+        <v>3299</v>
+      </c>
+      <c r="BD124" s="245"/>
+      <c r="BE124" s="245"/>
+      <c r="BF124" s="246"/>
       <c r="BG124" s="214" t="s">
         <v>367</v>
       </c>
@@ -36574,7 +36574,7 @@
         <v>1880</v>
       </c>
       <c r="D125" s="227" t="s">
-        <v>3317</v>
+        <v>3312</v>
       </c>
       <c r="E125" s="54" t="s">
         <v>1988</v>
@@ -36661,21 +36661,21 @@
       </c>
       <c r="AX125" s="243"/>
       <c r="AY125" s="226" t="s">
-        <v>3305</v>
-      </c>
-      <c r="AZ125" s="248" t="s">
-        <v>3305</v>
-      </c>
-      <c r="BA125" s="249"/>
+        <v>3300</v>
+      </c>
+      <c r="AZ125" s="244" t="s">
+        <v>3300</v>
+      </c>
+      <c r="BA125" s="246"/>
       <c r="BB125" s="177" t="s">
-        <v>3243</v>
-      </c>
-      <c r="BC125" s="248" t="s">
-        <v>3306</v>
-      </c>
-      <c r="BD125" s="250"/>
-      <c r="BE125" s="250"/>
-      <c r="BF125" s="249"/>
+        <v>3238</v>
+      </c>
+      <c r="BC125" s="244" t="s">
+        <v>3301</v>
+      </c>
+      <c r="BD125" s="245"/>
+      <c r="BE125" s="245"/>
+      <c r="BF125" s="246"/>
       <c r="BG125" s="214" t="s">
         <v>367</v>
       </c>
@@ -36896,25 +36896,25 @@
       <c r="AS127" s="67"/>
       <c r="AT127" s="147"/>
       <c r="AU127" s="133" t="s">
-        <v>3452</v>
+        <v>3447</v>
       </c>
       <c r="AV127" s="97"/>
       <c r="AW127" s="142" t="s">
         <v>367</v>
       </c>
       <c r="AX127" s="241" t="s">
-        <v>3446</v>
+        <v>3441</v>
       </c>
       <c r="AY127" s="241"/>
       <c r="AZ127" s="242" t="s">
-        <v>3446</v>
+        <v>3441</v>
       </c>
       <c r="BA127" s="242"/>
       <c r="BB127" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC127" s="242" t="s">
-        <v>3447</v>
+        <v>3442</v>
       </c>
       <c r="BD127" s="242"/>
       <c r="BE127" s="242"/>
@@ -37021,7 +37021,7 @@
       <c r="AS128" s="67"/>
       <c r="AT128" s="147"/>
       <c r="AU128" s="133" t="s">
-        <v>3451</v>
+        <v>3446</v>
       </c>
       <c r="AV128" s="97"/>
       <c r="AW128" s="243" t="s">
@@ -37029,22 +37029,22 @@
       </c>
       <c r="AX128" s="243"/>
       <c r="AY128" s="191" t="s">
-        <v>3449</v>
+        <v>3444</v>
       </c>
       <c r="AZ128" s="177" t="s">
-        <v>3449</v>
+        <v>3444</v>
       </c>
       <c r="BA128" s="177" t="s">
-        <v>3449</v>
+        <v>3444</v>
       </c>
       <c r="BB128" s="177" t="s">
-        <v>3243</v>
-      </c>
-      <c r="BC128" s="357" t="s">
-        <v>3450</v>
-      </c>
-      <c r="BD128" s="358"/>
-      <c r="BE128" s="359"/>
+        <v>3238</v>
+      </c>
+      <c r="BC128" s="354" t="s">
+        <v>3445</v>
+      </c>
+      <c r="BD128" s="355"/>
+      <c r="BE128" s="356"/>
       <c r="BF128" s="177"/>
       <c r="BG128" s="214" t="s">
         <v>367</v>
@@ -37163,7 +37163,7 @@
         <v>2906</v>
       </c>
       <c r="BB129" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC129" s="177" t="s">
         <v>2907</v>
@@ -37294,7 +37294,7 @@
         <v>2908</v>
       </c>
       <c r="BB130" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC130" s="177" t="s">
         <v>2909</v>
@@ -37425,7 +37425,7 @@
         <v>2910</v>
       </c>
       <c r="BB131" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC131" s="177" t="s">
         <v>2911</v>
@@ -38081,18 +38081,18 @@
       <c r="AY136" s="143" t="s">
         <v>3062</v>
       </c>
-      <c r="AZ136" s="244" t="s">
+      <c r="AZ136" s="247" t="s">
         <v>3062</v>
       </c>
-      <c r="BA136" s="244"/>
+      <c r="BA136" s="247"/>
       <c r="BB136" s="179" t="s">
         <v>3063</v>
       </c>
-      <c r="BC136" s="244" t="s">
+      <c r="BC136" s="247" t="s">
         <v>3064</v>
       </c>
-      <c r="BD136" s="244"/>
-      <c r="BE136" s="244"/>
+      <c r="BD136" s="247"/>
+      <c r="BE136" s="247"/>
       <c r="BF136" s="175" t="s">
         <v>367</v>
       </c>
@@ -38214,18 +38214,18 @@
       <c r="AY137" s="142" t="s">
         <v>3065</v>
       </c>
-      <c r="AZ137" s="244" t="s">
+      <c r="AZ137" s="247" t="s">
         <v>3065</v>
       </c>
-      <c r="BA137" s="244"/>
+      <c r="BA137" s="247"/>
       <c r="BB137" s="179" t="s">
         <v>3066</v>
       </c>
-      <c r="BC137" s="244" t="s">
+      <c r="BC137" s="247" t="s">
         <v>3067</v>
       </c>
-      <c r="BD137" s="244"/>
-      <c r="BE137" s="244"/>
+      <c r="BD137" s="247"/>
+      <c r="BE137" s="247"/>
       <c r="BF137" s="175" t="s">
         <v>367</v>
       </c>
@@ -38480,18 +38480,18 @@
       <c r="AY139" s="142" t="s">
         <v>3071</v>
       </c>
-      <c r="AZ139" s="244" t="s">
+      <c r="AZ139" s="247" t="s">
         <v>3071</v>
       </c>
-      <c r="BA139" s="244"/>
+      <c r="BA139" s="247"/>
       <c r="BB139" s="179" t="s">
         <v>3072</v>
       </c>
-      <c r="BC139" s="244" t="s">
+      <c r="BC139" s="247" t="s">
         <v>3073</v>
       </c>
-      <c r="BD139" s="244"/>
-      <c r="BE139" s="244"/>
+      <c r="BD139" s="247"/>
+      <c r="BE139" s="247"/>
       <c r="BF139" s="175" t="s">
         <v>367</v>
       </c>
@@ -38622,11 +38622,11 @@
       <c r="BB140" s="179" t="s">
         <v>3075</v>
       </c>
-      <c r="BC140" s="244" t="s">
+      <c r="BC140" s="247" t="s">
         <v>3076</v>
       </c>
-      <c r="BD140" s="244"/>
-      <c r="BE140" s="244"/>
+      <c r="BD140" s="247"/>
+      <c r="BE140" s="247"/>
       <c r="BF140" s="175" t="s">
         <v>367</v>
       </c>
@@ -38721,7 +38721,7 @@
         <v>367</v>
       </c>
       <c r="BB141" s="179" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC141" s="175" t="s">
         <v>3078</v>
@@ -38826,7 +38826,7 @@
         <v>367</v>
       </c>
       <c r="BB142" s="179" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC142" s="141" t="s">
         <v>3080</v>
@@ -38931,7 +38931,7 @@
         <v>367</v>
       </c>
       <c r="BB143" s="179" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC143" s="141" t="s">
         <v>3082</v>
@@ -39359,26 +39359,26 @@
       </c>
       <c r="AX146" s="243"/>
       <c r="AY146" s="142" t="s">
-        <v>3232</v>
+        <v>3227</v>
       </c>
       <c r="AZ146" s="234" t="s">
-        <v>3233</v>
+        <v>3228</v>
       </c>
       <c r="BA146" s="234"/>
       <c r="BB146" s="177" t="s">
         <v>3083</v>
       </c>
       <c r="BC146" s="234" t="s">
-        <v>3234</v>
+        <v>3229</v>
       </c>
       <c r="BD146" s="234"/>
       <c r="BE146" s="234"/>
       <c r="BF146" s="234"/>
       <c r="BG146" s="136" t="s">
-        <v>3235</v>
+        <v>3230</v>
       </c>
       <c r="BH146" s="236" t="s">
-        <v>3236</v>
+        <v>3231</v>
       </c>
       <c r="BI146" s="237"/>
       <c r="BJ146" s="237"/>
@@ -39514,26 +39514,26 @@
       </c>
       <c r="AX147" s="243"/>
       <c r="AY147" s="142" t="s">
-        <v>3328</v>
+        <v>3323</v>
       </c>
       <c r="AZ147" s="234" t="s">
-        <v>3328</v>
+        <v>3323</v>
       </c>
       <c r="BA147" s="234"/>
       <c r="BB147" s="177" t="s">
         <v>3084</v>
       </c>
       <c r="BC147" s="234" t="s">
-        <v>3329</v>
+        <v>3324</v>
       </c>
       <c r="BD147" s="234"/>
       <c r="BE147" s="234"/>
       <c r="BF147" s="234"/>
       <c r="BG147" s="136" t="s">
-        <v>3330</v>
+        <v>3325</v>
       </c>
       <c r="BH147" s="236" t="s">
-        <v>3331</v>
+        <v>3326</v>
       </c>
       <c r="BI147" s="237"/>
       <c r="BJ147" s="237"/>
@@ -39669,26 +39669,26 @@
       </c>
       <c r="AX148" s="243"/>
       <c r="AY148" s="142" t="s">
-        <v>3327</v>
+        <v>3322</v>
       </c>
       <c r="AZ148" s="234" t="s">
-        <v>3327</v>
+        <v>3322</v>
       </c>
       <c r="BA148" s="234"/>
       <c r="BB148" s="177" t="s">
         <v>3085</v>
       </c>
       <c r="BC148" s="234" t="s">
-        <v>3324</v>
+        <v>3319</v>
       </c>
       <c r="BD148" s="234"/>
       <c r="BE148" s="234"/>
       <c r="BF148" s="234"/>
       <c r="BG148" s="136" t="s">
-        <v>3325</v>
+        <v>3320</v>
       </c>
       <c r="BH148" s="236" t="s">
-        <v>3326</v>
+        <v>3321</v>
       </c>
       <c r="BI148" s="237"/>
       <c r="BJ148" s="237"/>
@@ -39953,7 +39953,7 @@
       <c r="AS150" s="67"/>
       <c r="AT150" s="147"/>
       <c r="AU150" s="133" t="s">
-        <v>3333</v>
+        <v>3328</v>
       </c>
       <c r="AV150" s="96" t="s">
         <v>2676</v>
@@ -39964,23 +39964,23 @@
       <c r="AX150" s="233"/>
       <c r="AY150" s="233"/>
       <c r="AZ150" s="234" t="s">
-        <v>3280</v>
+        <v>3275</v>
       </c>
       <c r="BA150" s="234"/>
       <c r="BB150" s="177" t="s">
-        <v>3281</v>
+        <v>3276</v>
       </c>
       <c r="BC150" s="234" t="s">
-        <v>3282</v>
+        <v>3277</v>
       </c>
       <c r="BD150" s="234"/>
       <c r="BE150" s="234"/>
       <c r="BF150" s="234"/>
       <c r="BG150" s="136" t="s">
-        <v>3283</v>
+        <v>3278</v>
       </c>
       <c r="BH150" s="236" t="s">
-        <v>3284</v>
+        <v>3279</v>
       </c>
       <c r="BI150" s="237"/>
       <c r="BJ150" s="237"/>
@@ -40108,7 +40108,7 @@
       <c r="AS151" s="67"/>
       <c r="AT151" s="147"/>
       <c r="AU151" s="133" t="s">
-        <v>3334</v>
+        <v>3329</v>
       </c>
       <c r="AV151" s="96" t="s">
         <v>2678</v>
@@ -40119,23 +40119,23 @@
       <c r="AX151" s="233"/>
       <c r="AY151" s="233"/>
       <c r="AZ151" s="331" t="s">
-        <v>3271</v>
+        <v>3266</v>
       </c>
       <c r="BA151" s="332"/>
       <c r="BB151" s="225" t="s">
-        <v>3272</v>
+        <v>3267</v>
       </c>
       <c r="BC151" s="234" t="s">
-        <v>3273</v>
+        <v>3268</v>
       </c>
       <c r="BD151" s="234"/>
       <c r="BE151" s="234"/>
       <c r="BF151" s="234"/>
       <c r="BG151" s="136" t="s">
-        <v>3274</v>
+        <v>3269</v>
       </c>
       <c r="BH151" s="236" t="s">
-        <v>3275</v>
+        <v>3270</v>
       </c>
       <c r="BI151" s="237"/>
       <c r="BJ151" s="237"/>
@@ -40263,7 +40263,7 @@
       <c r="AS152" s="67"/>
       <c r="AT152" s="147"/>
       <c r="AU152" s="133" t="s">
-        <v>3334</v>
+        <v>3329</v>
       </c>
       <c r="AV152" s="96" t="s">
         <v>2680</v>
@@ -40273,23 +40273,23 @@
       </c>
       <c r="AX152" s="233"/>
       <c r="AY152" s="142" t="s">
-        <v>3276</v>
+        <v>3271</v>
       </c>
       <c r="AZ152" s="234" t="s">
-        <v>3276</v>
+        <v>3271</v>
       </c>
       <c r="BA152" s="234"/>
       <c r="BB152" s="177" t="s">
-        <v>3277</v>
+        <v>3272</v>
       </c>
       <c r="BC152" s="234" t="s">
-        <v>3278</v>
+        <v>3273</v>
       </c>
       <c r="BD152" s="234"/>
       <c r="BE152" s="234"/>
       <c r="BF152" s="234"/>
       <c r="BG152" s="136" t="s">
-        <v>3279</v>
+        <v>3274</v>
       </c>
       <c r="BH152" s="236" t="s">
         <v>1839</v>
@@ -40420,7 +40420,7 @@
       <c r="AS153" s="67"/>
       <c r="AT153" s="147"/>
       <c r="AU153" s="133" t="s">
-        <v>3334</v>
+        <v>3329</v>
       </c>
       <c r="AV153" s="96" t="s">
         <v>2682</v>
@@ -40430,23 +40430,23 @@
       </c>
       <c r="AX153" s="233"/>
       <c r="AY153" s="142" t="s">
-        <v>3285</v>
+        <v>3280</v>
       </c>
       <c r="AZ153" s="234" t="s">
-        <v>3285</v>
+        <v>3280</v>
       </c>
       <c r="BA153" s="234"/>
       <c r="BB153" s="141" t="s">
-        <v>3286</v>
+        <v>3281</v>
       </c>
       <c r="BC153" s="234" t="s">
-        <v>3287</v>
+        <v>3282</v>
       </c>
       <c r="BD153" s="234"/>
       <c r="BE153" s="234"/>
       <c r="BF153" s="234"/>
       <c r="BG153" s="136" t="s">
-        <v>3288</v>
+        <v>3283</v>
       </c>
       <c r="BH153" s="236" t="s">
         <v>1840</v>
@@ -40577,7 +40577,7 @@
       <c r="AS154" s="67"/>
       <c r="AT154" s="147"/>
       <c r="AU154" s="133" t="s">
-        <v>3334</v>
+        <v>3329</v>
       </c>
       <c r="AV154" s="96" t="s">
         <v>2684</v>
@@ -40587,26 +40587,26 @@
       </c>
       <c r="AX154" s="233"/>
       <c r="AY154" s="142" t="s">
-        <v>3319</v>
+        <v>3314</v>
       </c>
       <c r="AZ154" s="234" t="s">
-        <v>3319</v>
+        <v>3314</v>
       </c>
       <c r="BA154" s="234"/>
       <c r="BB154" s="141" t="s">
-        <v>3241</v>
+        <v>3236</v>
       </c>
       <c r="BC154" s="234" t="s">
-        <v>3320</v>
+        <v>3315</v>
       </c>
       <c r="BD154" s="234"/>
       <c r="BE154" s="234"/>
       <c r="BF154" s="234"/>
       <c r="BG154" s="136" t="s">
-        <v>3321</v>
+        <v>3316</v>
       </c>
       <c r="BH154" s="236" t="s">
-        <v>3322</v>
+        <v>3317</v>
       </c>
       <c r="BI154" s="237"/>
       <c r="BJ154" s="237"/>
@@ -40734,7 +40734,7 @@
       <c r="AS155" s="67"/>
       <c r="AT155" s="147"/>
       <c r="AU155" s="133" t="s">
-        <v>3334</v>
+        <v>3329</v>
       </c>
       <c r="AV155" s="96" t="s">
         <v>2686</v>
@@ -40744,26 +40744,26 @@
       </c>
       <c r="AX155" s="233"/>
       <c r="AY155" s="142" t="s">
-        <v>3290</v>
+        <v>3285</v>
       </c>
       <c r="AZ155" s="234" t="s">
-        <v>3290</v>
+        <v>3285</v>
       </c>
       <c r="BA155" s="234"/>
       <c r="BB155" s="141" t="s">
-        <v>3291</v>
+        <v>3286</v>
       </c>
       <c r="BC155" s="234" t="s">
-        <v>3292</v>
+        <v>3287</v>
       </c>
       <c r="BD155" s="234"/>
       <c r="BE155" s="234"/>
       <c r="BF155" s="234"/>
       <c r="BG155" s="136" t="s">
-        <v>3289</v>
+        <v>3284</v>
       </c>
       <c r="BH155" s="236" t="s">
-        <v>3323</v>
+        <v>3318</v>
       </c>
       <c r="BI155" s="237"/>
       <c r="BJ155" s="237"/>
@@ -42143,7 +42143,7 @@
       </c>
       <c r="AX166" s="233"/>
       <c r="AY166" s="143" t="s">
-        <v>3242</v>
+        <v>3237</v>
       </c>
       <c r="AZ166" s="234" t="s">
         <v>3101</v>
@@ -42439,17 +42439,17 @@
       </c>
       <c r="AX168" s="233"/>
       <c r="AY168" s="142" t="s">
-        <v>3239</v>
+        <v>3234</v>
       </c>
       <c r="AZ168" s="234" t="s">
-        <v>3239</v>
+        <v>3234</v>
       </c>
       <c r="BA168" s="234"/>
       <c r="BB168" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC168" s="234" t="s">
-        <v>3240</v>
+        <v>3235</v>
       </c>
       <c r="BD168" s="234"/>
       <c r="BE168" s="234"/>
@@ -42585,7 +42585,7 @@
       </c>
       <c r="BA169" s="234"/>
       <c r="BB169" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC169" s="234" t="s">
         <v>3105</v>
@@ -42724,7 +42724,7 @@
       </c>
       <c r="BA170" s="234"/>
       <c r="BB170" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC170" s="234" t="s">
         <v>3108</v>
@@ -43208,7 +43208,7 @@
       </c>
       <c r="BA174" s="234"/>
       <c r="BB174" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC174" s="234" t="s">
         <v>3115</v>
@@ -43465,19 +43465,19 @@
         <v>2912</v>
       </c>
       <c r="AW176" s="243" t="s">
-        <v>3116</v>
+        <v>3467</v>
       </c>
       <c r="AX176" s="243"/>
       <c r="AY176" s="243"/>
       <c r="AZ176" s="234" t="s">
-        <v>3117</v>
+        <v>3466</v>
       </c>
       <c r="BA176" s="234"/>
       <c r="BB176" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC176" s="234" t="s">
-        <v>3118</v>
+        <v>3465</v>
       </c>
       <c r="BD176" s="234"/>
       <c r="BE176" s="234"/>
@@ -43604,19 +43604,19 @@
         <v>2437</v>
       </c>
       <c r="AW177" s="243" t="s">
-        <v>3119</v>
+        <v>3116</v>
       </c>
       <c r="AX177" s="243"/>
       <c r="AY177" s="243"/>
       <c r="AZ177" s="234" t="s">
-        <v>3120</v>
+        <v>3117</v>
       </c>
       <c r="BA177" s="234"/>
       <c r="BB177" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC177" s="234" t="s">
-        <v>3121</v>
+        <v>3118</v>
       </c>
       <c r="BD177" s="234"/>
       <c r="BE177" s="234"/>
@@ -43743,19 +43743,19 @@
         <v>2725</v>
       </c>
       <c r="AW178" s="243" t="s">
-        <v>3122</v>
+        <v>3119</v>
       </c>
       <c r="AX178" s="243"/>
       <c r="AY178" s="243"/>
       <c r="AZ178" s="234" t="s">
-        <v>3123</v>
+        <v>3120</v>
       </c>
       <c r="BA178" s="234"/>
       <c r="BB178" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC178" s="234" t="s">
-        <v>3124</v>
+        <v>3121</v>
       </c>
       <c r="BD178" s="234"/>
       <c r="BE178" s="234"/>
@@ -43882,19 +43882,19 @@
         <v>2727</v>
       </c>
       <c r="AW179" s="243" t="s">
-        <v>3125</v>
+        <v>3122</v>
       </c>
       <c r="AX179" s="243"/>
       <c r="AY179" s="243"/>
       <c r="AZ179" s="234" t="s">
-        <v>3126</v>
+        <v>3123</v>
       </c>
       <c r="BA179" s="234"/>
       <c r="BB179" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC179" s="234" t="s">
-        <v>3127</v>
+        <v>3124</v>
       </c>
       <c r="BD179" s="234"/>
       <c r="BE179" s="234"/>
@@ -44019,19 +44019,19 @@
       <c r="AU180" s="133"/>
       <c r="AV180" s="96"/>
       <c r="AW180" s="243" t="s">
-        <v>3128</v>
+        <v>3463</v>
       </c>
       <c r="AX180" s="243"/>
       <c r="AY180" s="243"/>
       <c r="AZ180" s="234" t="s">
-        <v>3128</v>
+        <v>3463</v>
       </c>
       <c r="BA180" s="234"/>
       <c r="BB180" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC180" s="234" t="s">
-        <v>3129</v>
+        <v>3464</v>
       </c>
       <c r="BD180" s="234"/>
       <c r="BE180" s="234"/>
@@ -44158,19 +44158,19 @@
         <v>2730</v>
       </c>
       <c r="AW181" s="243" t="s">
-        <v>3130</v>
+        <v>3125</v>
       </c>
       <c r="AX181" s="243"/>
       <c r="AY181" s="243"/>
       <c r="AZ181" s="234" t="s">
-        <v>3130</v>
+        <v>3125</v>
       </c>
       <c r="BA181" s="234"/>
       <c r="BB181" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC181" s="234" t="s">
-        <v>3131</v>
+        <v>3126</v>
       </c>
       <c r="BD181" s="234"/>
       <c r="BE181" s="234"/>
@@ -44297,19 +44297,19 @@
         <v>2732</v>
       </c>
       <c r="AW182" s="243" t="s">
-        <v>3132</v>
+        <v>3127</v>
       </c>
       <c r="AX182" s="243"/>
       <c r="AY182" s="243"/>
       <c r="AZ182" s="234" t="s">
-        <v>3133</v>
+        <v>3128</v>
       </c>
       <c r="BA182" s="234"/>
       <c r="BB182" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC182" s="234" t="s">
-        <v>3134</v>
+        <v>3129</v>
       </c>
       <c r="BD182" s="234"/>
       <c r="BE182" s="234"/>
@@ -44539,17 +44539,17 @@
       </c>
       <c r="AX184" s="243"/>
       <c r="AY184" s="142" t="s">
-        <v>3135</v>
+        <v>3130</v>
       </c>
       <c r="AZ184" s="234" t="s">
-        <v>3135</v>
+        <v>3130</v>
       </c>
       <c r="BA184" s="234"/>
       <c r="BB184" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC184" s="234" t="s">
-        <v>3136</v>
+        <v>3131</v>
       </c>
       <c r="BD184" s="234"/>
       <c r="BE184" s="234"/>
@@ -44668,17 +44668,17 @@
       </c>
       <c r="AX185" s="243"/>
       <c r="AY185" s="142" t="s">
-        <v>3137</v>
+        <v>3132</v>
       </c>
       <c r="AZ185" s="234" t="s">
-        <v>3137</v>
+        <v>3132</v>
       </c>
       <c r="BA185" s="234"/>
       <c r="BB185" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC185" s="234" t="s">
-        <v>3138</v>
+        <v>3133</v>
       </c>
       <c r="BD185" s="234"/>
       <c r="BE185" s="234"/>
@@ -44797,17 +44797,17 @@
       </c>
       <c r="AX186" s="243"/>
       <c r="AY186" s="142" t="s">
-        <v>3139</v>
+        <v>3134</v>
       </c>
       <c r="AZ186" s="234" t="s">
-        <v>3139</v>
+        <v>3134</v>
       </c>
       <c r="BA186" s="234"/>
       <c r="BB186" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC186" s="234" t="s">
-        <v>3140</v>
+        <v>3135</v>
       </c>
       <c r="BD186" s="234"/>
       <c r="BE186" s="234"/>
@@ -44926,17 +44926,17 @@
       </c>
       <c r="AX187" s="243"/>
       <c r="AY187" s="142" t="s">
-        <v>3141</v>
+        <v>3136</v>
       </c>
       <c r="AZ187" s="234" t="s">
-        <v>3141</v>
+        <v>3136</v>
       </c>
       <c r="BA187" s="234"/>
       <c r="BB187" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC187" s="234" t="s">
-        <v>3142</v>
+        <v>3137</v>
       </c>
       <c r="BD187" s="234"/>
       <c r="BE187" s="234"/>
@@ -45055,17 +45055,17 @@
       </c>
       <c r="AX188" s="243"/>
       <c r="AY188" s="142" t="s">
-        <v>3143</v>
+        <v>3138</v>
       </c>
       <c r="AZ188" s="234" t="s">
-        <v>3143</v>
+        <v>3138</v>
       </c>
       <c r="BA188" s="234"/>
       <c r="BB188" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC188" s="234" t="s">
-        <v>3144</v>
+        <v>3139</v>
       </c>
       <c r="BD188" s="234"/>
       <c r="BE188" s="234"/>
@@ -45174,17 +45174,17 @@
       </c>
       <c r="AX189" s="243"/>
       <c r="AY189" s="142" t="s">
-        <v>3145</v>
+        <v>3140</v>
       </c>
       <c r="AZ189" s="234" t="s">
-        <v>3210</v>
+        <v>3205</v>
       </c>
       <c r="BA189" s="234"/>
       <c r="BB189" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC189" s="234" t="s">
-        <v>3146</v>
+        <v>3141</v>
       </c>
       <c r="BD189" s="234"/>
       <c r="BE189" s="234"/>
@@ -45305,17 +45305,17 @@
       </c>
       <c r="AX190" s="243"/>
       <c r="AY190" s="142" t="s">
-        <v>3147</v>
+        <v>3142</v>
       </c>
       <c r="AZ190" s="234" t="s">
-        <v>3147</v>
+        <v>3142</v>
       </c>
       <c r="BA190" s="234"/>
       <c r="BB190" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC190" s="234" t="s">
-        <v>3148</v>
+        <v>3143</v>
       </c>
       <c r="BD190" s="234"/>
       <c r="BE190" s="234"/>
@@ -45432,17 +45432,17 @@
       </c>
       <c r="AX191" s="243"/>
       <c r="AY191" s="142" t="s">
-        <v>3149</v>
+        <v>3144</v>
       </c>
       <c r="AZ191" s="234" t="s">
-        <v>3149</v>
+        <v>3144</v>
       </c>
       <c r="BA191" s="234"/>
       <c r="BB191" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC191" s="234" t="s">
-        <v>3150</v>
+        <v>3145</v>
       </c>
       <c r="BD191" s="234"/>
       <c r="BE191" s="234"/>
@@ -45559,17 +45559,17 @@
       </c>
       <c r="AX192" s="243"/>
       <c r="AY192" s="142" t="s">
-        <v>3151</v>
+        <v>3146</v>
       </c>
       <c r="AZ192" s="234" t="s">
-        <v>3151</v>
+        <v>3146</v>
       </c>
       <c r="BA192" s="234"/>
       <c r="BB192" s="177" t="s">
         <v>367</v>
       </c>
       <c r="BC192" s="234" t="s">
-        <v>3150</v>
+        <v>3145</v>
       </c>
       <c r="BD192" s="234"/>
       <c r="BE192" s="234"/>
@@ -45667,7 +45667,7 @@
       <c r="AX193" s="243"/>
       <c r="AY193" s="243"/>
       <c r="AZ193" s="234" t="s">
-        <v>3152</v>
+        <v>3147</v>
       </c>
       <c r="BA193" s="234"/>
       <c r="BB193" s="177" t="s">
@@ -45677,7 +45677,7 @@
         <v>367</v>
       </c>
       <c r="BD193" s="141" t="s">
-        <v>3153</v>
+        <v>3148</v>
       </c>
       <c r="BE193" s="141" t="s">
         <v>367</v>
@@ -45785,7 +45785,7 @@
       </c>
       <c r="AX194" s="243"/>
       <c r="AY194" s="142" t="s">
-        <v>3154</v>
+        <v>3149</v>
       </c>
       <c r="AZ194" s="234" t="s">
         <v>367</v>
@@ -45795,7 +45795,7 @@
         <v>367</v>
       </c>
       <c r="BC194" s="234" t="s">
-        <v>3155</v>
+        <v>3150</v>
       </c>
       <c r="BD194" s="234"/>
       <c r="BE194" s="234"/>
@@ -45902,7 +45902,7 @@
       </c>
       <c r="AX195" s="243"/>
       <c r="AY195" s="142" t="s">
-        <v>3156</v>
+        <v>3151</v>
       </c>
       <c r="AZ195" s="234" t="s">
         <v>367</v>
@@ -45912,7 +45912,7 @@
         <v>367</v>
       </c>
       <c r="BC195" s="234" t="s">
-        <v>3157</v>
+        <v>3152</v>
       </c>
       <c r="BD195" s="234"/>
       <c r="BE195" s="234"/>
@@ -46011,7 +46011,7 @@
         <v>367</v>
       </c>
       <c r="BC196" s="234" t="s">
-        <v>3448</v>
+        <v>3443</v>
       </c>
       <c r="BD196" s="234"/>
       <c r="BE196" s="234" t="s">
@@ -46128,17 +46128,17 @@
       </c>
       <c r="AX197" s="243"/>
       <c r="AY197" s="142" t="s">
-        <v>3158</v>
+        <v>3153</v>
       </c>
       <c r="AZ197" s="234" t="s">
-        <v>3159</v>
+        <v>3154</v>
       </c>
       <c r="BA197" s="234"/>
       <c r="BB197" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC197" s="234" t="s">
-        <v>3160</v>
+        <v>3155</v>
       </c>
       <c r="BD197" s="234"/>
       <c r="BE197" s="234"/>
@@ -46255,17 +46255,17 @@
       </c>
       <c r="AX198" s="243"/>
       <c r="AY198" s="142" t="s">
-        <v>3161</v>
+        <v>3156</v>
       </c>
       <c r="AZ198" s="234" t="s">
-        <v>3162</v>
+        <v>3157</v>
       </c>
       <c r="BA198" s="234"/>
       <c r="BB198" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC198" s="234" t="s">
-        <v>3163</v>
+        <v>3158</v>
       </c>
       <c r="BD198" s="234"/>
       <c r="BE198" s="234"/>
@@ -46354,7 +46354,7 @@
       </c>
       <c r="AX199" s="243"/>
       <c r="AY199" s="142" t="s">
-        <v>3164</v>
+        <v>3159</v>
       </c>
       <c r="AZ199" s="234" t="s">
         <v>367</v>
@@ -46364,7 +46364,7 @@
         <v>367</v>
       </c>
       <c r="BC199" s="141" t="s">
-        <v>3165</v>
+        <v>3160</v>
       </c>
       <c r="BD199" s="234" t="s">
         <v>367</v>
@@ -46465,7 +46465,7 @@
         <v>367</v>
       </c>
       <c r="BC200" s="234" t="s">
-        <v>3166</v>
+        <v>3161</v>
       </c>
       <c r="BD200" s="234"/>
       <c r="BE200" s="234" t="s">
@@ -46566,7 +46566,7 @@
         <v>367</v>
       </c>
       <c r="BC201" s="234" t="s">
-        <v>3167</v>
+        <v>3162</v>
       </c>
       <c r="BD201" s="234"/>
       <c r="BE201" s="234" t="s">
@@ -46667,7 +46667,7 @@
         <v>367</v>
       </c>
       <c r="BC202" s="234" t="s">
-        <v>3168</v>
+        <v>3163</v>
       </c>
       <c r="BD202" s="234"/>
       <c r="BE202" s="234" t="s">
@@ -46786,24 +46786,24 @@
       </c>
       <c r="AX203" s="243"/>
       <c r="AY203" s="142" t="s">
-        <v>3169</v>
+        <v>3164</v>
       </c>
       <c r="AZ203" s="234" t="s">
-        <v>3169</v>
+        <v>3164</v>
       </c>
       <c r="BA203" s="234"/>
       <c r="BB203" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC203" s="234" t="s">
-        <v>3170</v>
+        <v>3165</v>
       </c>
       <c r="BD203" s="234"/>
       <c r="BE203" s="141" t="s">
         <v>367</v>
       </c>
       <c r="BF203" s="141" t="s">
-        <v>3170</v>
+        <v>3165</v>
       </c>
       <c r="BG203" s="214" t="s">
         <v>367</v>
@@ -46917,24 +46917,24 @@
       </c>
       <c r="AX204" s="243"/>
       <c r="AY204" s="142" t="s">
-        <v>3171</v>
+        <v>3166</v>
       </c>
       <c r="AZ204" s="234" t="s">
-        <v>3171</v>
+        <v>3166</v>
       </c>
       <c r="BA204" s="234"/>
       <c r="BB204" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC204" s="234" t="s">
-        <v>3172</v>
+        <v>3167</v>
       </c>
       <c r="BD204" s="234"/>
       <c r="BE204" s="141" t="s">
         <v>367</v>
       </c>
       <c r="BF204" s="141" t="s">
-        <v>3172</v>
+        <v>3167</v>
       </c>
       <c r="BG204" s="214" t="s">
         <v>367</v>
@@ -47155,7 +47155,7 @@
       <c r="BE206" s="234"/>
       <c r="BF206" s="234"/>
       <c r="BG206" s="136" t="s">
-        <v>3256</v>
+        <v>3251</v>
       </c>
       <c r="BH206" s="293" t="s">
         <v>2890</v>
@@ -47165,7 +47165,7 @@
         <v>367</v>
       </c>
       <c r="BK206" s="201" t="s">
-        <v>3257</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="207" spans="1:63" ht="189.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47264,7 +47264,7 @@
       <c r="BE207" s="234"/>
       <c r="BF207" s="234"/>
       <c r="BG207" s="136" t="s">
-        <v>3259</v>
+        <v>3254</v>
       </c>
       <c r="BH207" s="293" t="s">
         <v>1797</v>
@@ -47274,7 +47274,7 @@
         <v>367</v>
       </c>
       <c r="BK207" s="201" t="s">
-        <v>3258</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="208" spans="1:63" s="144" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -48296,7 +48296,7 @@
       <c r="AS217" s="67"/>
       <c r="AT217" s="147"/>
       <c r="AU217" s="133" t="s">
-        <v>3312</v>
+        <v>3307</v>
       </c>
       <c r="AV217" s="96"/>
       <c r="AW217" s="243" t="s">
@@ -48317,7 +48317,7 @@
         <v>367</v>
       </c>
       <c r="BH217" s="346" t="s">
-        <v>3311</v>
+        <v>3306</v>
       </c>
       <c r="BI217" s="240" t="s">
         <v>367</v>
@@ -49059,15 +49059,15 @@
       <c r="BE224" s="234"/>
       <c r="BF224" s="234"/>
       <c r="BG224" s="136" t="s">
-        <v>3309</v>
+        <v>3304</v>
       </c>
       <c r="BH224" s="240" t="s">
-        <v>3308</v>
+        <v>3303</v>
       </c>
       <c r="BI224" s="240"/>
       <c r="BJ224" s="240"/>
       <c r="BK224" s="201" t="s">
-        <v>3310</v>
+        <v>3305</v>
       </c>
     </row>
     <row r="225" spans="1:63" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -51024,8 +51024,8 @@
       <c r="BH242" s="295" t="s">
         <v>2061</v>
       </c>
-      <c r="BI242" s="354"/>
-      <c r="BJ242" s="354"/>
+      <c r="BI242" s="357"/>
+      <c r="BJ242" s="357"/>
       <c r="BK242" s="201" t="s">
         <v>2242</v>
       </c>
@@ -51102,16 +51102,16 @@
       <c r="AS243" s="67"/>
       <c r="AT243" s="147"/>
       <c r="AU243" s="131" t="s">
-        <v>3336</v>
+        <v>3331</v>
       </c>
       <c r="AV243" s="129" t="s">
         <v>2075</v>
       </c>
-      <c r="AW243" s="247" t="s">
-        <v>367</v>
-      </c>
-      <c r="AX243" s="247"/>
-      <c r="AY243" s="247"/>
+      <c r="AW243" s="250" t="s">
+        <v>367</v>
+      </c>
+      <c r="AX243" s="250"/>
+      <c r="AY243" s="250"/>
       <c r="AZ243" s="234" t="s">
         <v>367</v>
       </c>
@@ -51125,9 +51125,9 @@
         <v>367</v>
       </c>
       <c r="BH243" s="295" t="s">
-        <v>3335</v>
-      </c>
-      <c r="BI243" s="354"/>
+        <v>3330</v>
+      </c>
+      <c r="BI243" s="357"/>
       <c r="BJ243" s="198" t="s">
         <v>367</v>
       </c>
@@ -51217,7 +51217,7 @@
         <v>377</v>
       </c>
       <c r="AU244" s="130" t="s">
-        <v>3262</v>
+        <v>3257</v>
       </c>
       <c r="AV244" s="129"/>
       <c r="AW244" s="243" t="s">
@@ -51238,12 +51238,12 @@
         <v>367</v>
       </c>
       <c r="BH244" s="240" t="s">
-        <v>3254</v>
+        <v>3249</v>
       </c>
       <c r="BI244" s="239"/>
       <c r="BJ244" s="239"/>
       <c r="BK244" s="201" t="s">
-        <v>3255</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="245" spans="1:63" s="144" customFormat="1" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -51858,7 +51858,7 @@
         <v>237</v>
       </c>
       <c r="AU249" s="279" t="s">
-        <v>3268</v>
+        <v>3263</v>
       </c>
       <c r="AV249" s="129"/>
       <c r="AW249" s="243" t="s">
@@ -51873,7 +51873,7 @@
       </c>
       <c r="BA249" s="234"/>
       <c r="BB249" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC249" s="234" t="s">
         <v>2121</v>
@@ -52034,7 +52034,7 @@
       </c>
       <c r="BA250" s="234"/>
       <c r="BB250" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC250" s="234" t="s">
         <v>2124</v>
@@ -52191,14 +52191,14 @@
         <v>2383</v>
       </c>
       <c r="AZ251" s="234" t="s">
-        <v>3173</v>
+        <v>3168</v>
       </c>
       <c r="BA251" s="234"/>
       <c r="BB251" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC251" s="234" t="s">
-        <v>3174</v>
+        <v>3169</v>
       </c>
       <c r="BD251" s="234"/>
       <c r="BE251" s="234"/>
@@ -52352,14 +52352,14 @@
         <v>2387</v>
       </c>
       <c r="AZ252" s="234" t="s">
-        <v>3206</v>
+        <v>3201</v>
       </c>
       <c r="BA252" s="234"/>
       <c r="BB252" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC252" s="234" t="s">
-        <v>3206</v>
+        <v>3201</v>
       </c>
       <c r="BD252" s="242"/>
       <c r="BE252" s="242"/>
@@ -52513,14 +52513,14 @@
         <v>2388</v>
       </c>
       <c r="AZ253" s="234" t="s">
-        <v>3175</v>
+        <v>3170</v>
       </c>
       <c r="BA253" s="234"/>
       <c r="BB253" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC253" s="234" t="s">
-        <v>3176</v>
+        <v>3171</v>
       </c>
       <c r="BD253" s="234"/>
       <c r="BE253" s="234"/>
@@ -52678,7 +52678,7 @@
       </c>
       <c r="BA254" s="238"/>
       <c r="BB254" s="177" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC254" s="238" t="s">
         <v>2390</v>
@@ -52768,7 +52768,7 @@
         <v>0</v>
       </c>
       <c r="AU255" s="166" t="s">
-        <v>3263</v>
+        <v>3258</v>
       </c>
       <c r="AV255" s="129"/>
       <c r="AW255" s="243" t="s">
@@ -52869,7 +52869,7 @@
         <v>377</v>
       </c>
       <c r="AU256" s="58" t="s">
-        <v>3263</v>
+        <v>3258</v>
       </c>
       <c r="AV256" s="129"/>
       <c r="AW256" s="243" t="s">
@@ -53135,17 +53135,17 @@
       </c>
       <c r="AX258" s="243"/>
       <c r="AY258" s="178" t="s">
-        <v>3177</v>
+        <v>3172</v>
       </c>
       <c r="AZ258" s="234" t="s">
-        <v>3178</v>
+        <v>3173</v>
       </c>
       <c r="BA258" s="234"/>
       <c r="BB258" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC258" s="234" t="s">
-        <v>3179</v>
+        <v>3174</v>
       </c>
       <c r="BD258" s="234"/>
       <c r="BE258" s="234"/>
@@ -53296,17 +53296,17 @@
       </c>
       <c r="AX259" s="243"/>
       <c r="AY259" s="178" t="s">
-        <v>3180</v>
+        <v>3175</v>
       </c>
       <c r="AZ259" s="234" t="s">
-        <v>3181</v>
+        <v>3176</v>
       </c>
       <c r="BA259" s="234"/>
       <c r="BB259" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC259" s="234" t="s">
-        <v>3182</v>
+        <v>3177</v>
       </c>
       <c r="BD259" s="234"/>
       <c r="BE259" s="234"/>
@@ -53523,7 +53523,7 @@
         <v>367</v>
       </c>
       <c r="BH261" s="240" t="s">
-        <v>3245</v>
+        <v>3240</v>
       </c>
       <c r="BI261" s="240"/>
       <c r="BJ261" s="240"/>
@@ -53731,7 +53731,7 @@
         <v>367</v>
       </c>
       <c r="BH263" s="240" t="s">
-        <v>3244</v>
+        <v>3239</v>
       </c>
       <c r="BI263" s="240"/>
       <c r="BJ263" s="240"/>
@@ -53840,7 +53840,7 @@
         <v>367</v>
       </c>
       <c r="BH264" s="240" t="s">
-        <v>3246</v>
+        <v>3241</v>
       </c>
       <c r="BI264" s="240"/>
       <c r="BJ264" s="240"/>
@@ -54104,19 +54104,19 @@
       <c r="AW266" s="142" t="s">
         <v>367</v>
       </c>
-      <c r="AX266" s="246" t="s">
-        <v>3183</v>
-      </c>
-      <c r="AY266" s="246"/>
+      <c r="AX266" s="249" t="s">
+        <v>3178</v>
+      </c>
+      <c r="AY266" s="249"/>
       <c r="AZ266" s="234" t="s">
-        <v>3183</v>
+        <v>3178</v>
       </c>
       <c r="BA266" s="234"/>
       <c r="BB266" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC266" s="234" t="s">
-        <v>3184</v>
+        <v>3179</v>
       </c>
       <c r="BD266" s="234"/>
       <c r="BE266" s="234"/>
@@ -54237,21 +54237,21 @@
       <c r="AW267" s="142" t="s">
         <v>367</v>
       </c>
-      <c r="AX267" s="246" t="s">
-        <v>3211</v>
-      </c>
-      <c r="AY267" s="246"/>
+      <c r="AX267" s="249" t="s">
+        <v>3206</v>
+      </c>
+      <c r="AY267" s="249"/>
       <c r="AZ267" s="176" t="s">
-        <v>3185</v>
+        <v>3180</v>
       </c>
       <c r="BA267" s="141" t="s">
         <v>367</v>
       </c>
       <c r="BB267" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC267" s="141" t="s">
-        <v>3186</v>
+        <v>3181</v>
       </c>
       <c r="BD267" s="234" t="s">
         <v>367</v>
@@ -54378,7 +54378,7 @@
       <c r="AS268" s="71"/>
       <c r="AT268" s="157"/>
       <c r="AU268" s="158" t="s">
-        <v>3264</v>
+        <v>3259</v>
       </c>
       <c r="AV268" s="96"/>
       <c r="AW268" s="243" t="s">
@@ -54398,11 +54398,11 @@
       <c r="BG268" s="214" t="s">
         <v>367</v>
       </c>
-      <c r="BH268" s="355" t="s">
-        <v>3253</v>
-      </c>
-      <c r="BI268" s="356"/>
-      <c r="BJ268" s="356"/>
+      <c r="BH268" s="358" t="s">
+        <v>3248</v>
+      </c>
+      <c r="BI268" s="359"/>
+      <c r="BJ268" s="359"/>
       <c r="BK268" s="202" t="s">
         <v>367</v>
       </c>
@@ -54473,7 +54473,7 @@
       <c r="AS269" s="67"/>
       <c r="AT269" s="147"/>
       <c r="AU269" s="133" t="s">
-        <v>3265</v>
+        <v>3260</v>
       </c>
       <c r="AV269" s="96"/>
       <c r="AW269" s="243" t="s">
@@ -54496,7 +54496,7 @@
       <c r="BH269" s="295" t="s">
         <v>1794</v>
       </c>
-      <c r="BI269" s="354"/>
+      <c r="BI269" s="357"/>
       <c r="BJ269" s="198" t="s">
         <v>367</v>
       </c>
@@ -54646,19 +54646,19 @@
         <v>2856</v>
       </c>
       <c r="AW270" s="243" t="s">
-        <v>3187</v>
+        <v>3182</v>
       </c>
       <c r="AX270" s="243"/>
       <c r="AY270" s="243"/>
       <c r="AZ270" s="234" t="s">
-        <v>3188</v>
+        <v>3183</v>
       </c>
       <c r="BA270" s="234"/>
       <c r="BB270" s="222" t="s">
-        <v>3243</v>
+        <v>3238</v>
       </c>
       <c r="BC270" s="234" t="s">
-        <v>3189</v>
+        <v>3184</v>
       </c>
       <c r="BD270" s="234"/>
       <c r="BE270" s="234"/>
@@ -54852,7 +54852,7 @@
       <c r="AS272" s="67"/>
       <c r="AT272" s="147"/>
       <c r="AU272" s="133" t="s">
-        <v>3266</v>
+        <v>3261</v>
       </c>
       <c r="AV272" s="129"/>
       <c r="AW272" s="243" t="s">
@@ -54870,10 +54870,10 @@
       <c r="BE272" s="234"/>
       <c r="BF272" s="234"/>
       <c r="BG272" s="136" t="s">
-        <v>3249</v>
+        <v>3244</v>
       </c>
       <c r="BH272" s="240" t="s">
-        <v>3247</v>
+        <v>3242</v>
       </c>
       <c r="BI272" s="239"/>
       <c r="BJ272" s="198" t="s">
@@ -54979,10 +54979,10 @@
       <c r="BE273" s="234"/>
       <c r="BF273" s="234"/>
       <c r="BG273" s="219" t="s">
-        <v>3250</v>
+        <v>3245</v>
       </c>
       <c r="BH273" s="240" t="s">
-        <v>3248</v>
+        <v>3243</v>
       </c>
       <c r="BI273" s="239"/>
       <c r="BJ273" s="198" t="s">
@@ -55088,7 +55088,7 @@
       <c r="BE274" s="234"/>
       <c r="BF274" s="234"/>
       <c r="BG274" s="136" t="s">
-        <v>3251</v>
+        <v>3246</v>
       </c>
       <c r="BH274" s="240" t="s">
         <v>1795</v>
@@ -55181,7 +55181,7 @@
       <c r="AS275" s="67"/>
       <c r="AT275" s="147"/>
       <c r="AU275" s="133" t="s">
-        <v>3267</v>
+        <v>3262</v>
       </c>
       <c r="AV275" s="129"/>
       <c r="AW275" s="243" t="s">
@@ -55199,7 +55199,7 @@
       <c r="BE275" s="234"/>
       <c r="BF275" s="234"/>
       <c r="BG275" s="136" t="s">
-        <v>3252</v>
+        <v>3247</v>
       </c>
       <c r="BH275" s="240" t="s">
         <v>1796</v>
@@ -58012,6 +58012,7 @@
     <mergeCell ref="BC254:BF254"/>
     <mergeCell ref="AZ258:BA258"/>
     <mergeCell ref="AZ259:BA259"/>
+    <mergeCell ref="BH264:BJ264"/>
     <mergeCell ref="BH155:BJ155"/>
     <mergeCell ref="BH157:BI157"/>
     <mergeCell ref="BH239:BJ239"/>
@@ -58189,7 +58190,6 @@
     <mergeCell ref="A254:B254"/>
     <mergeCell ref="A255:B255"/>
     <mergeCell ref="BC31:BF31"/>
-    <mergeCell ref="BH264:BJ264"/>
     <mergeCell ref="BH250:BJ250"/>
     <mergeCell ref="BH251:BJ251"/>
     <mergeCell ref="BH252:BJ252"/>
@@ -58221,6 +58221,7 @@
     <mergeCell ref="BC152:BF152"/>
     <mergeCell ref="AW24:AY24"/>
     <mergeCell ref="AW25:AY25"/>
+    <mergeCell ref="AW91:AY91"/>
     <mergeCell ref="A309:B309"/>
     <mergeCell ref="A310:B310"/>
     <mergeCell ref="A311:B311"/>
@@ -58748,7 +58749,6 @@
     <mergeCell ref="BH173:BJ173"/>
     <mergeCell ref="BH23:BJ23"/>
     <mergeCell ref="BH22:BJ22"/>
-    <mergeCell ref="AW91:AY91"/>
     <mergeCell ref="AW101:AX101"/>
     <mergeCell ref="AW102:AX102"/>
     <mergeCell ref="AZ24:BA24"/>
@@ -58779,6 +58779,8 @@
     <mergeCell ref="BC52:BF52"/>
     <mergeCell ref="AZ52:BA52"/>
     <mergeCell ref="AZ63:BA63"/>
+    <mergeCell ref="AW93:AX93"/>
+    <mergeCell ref="AW94:AX94"/>
     <mergeCell ref="AZ147:BA147"/>
     <mergeCell ref="BC147:BF147"/>
     <mergeCell ref="BC148:BF148"/>
@@ -58907,8 +58909,6 @@
     <mergeCell ref="AW50:AY50"/>
     <mergeCell ref="AW51:AY51"/>
     <mergeCell ref="AW52:AY52"/>
-    <mergeCell ref="AW93:AX93"/>
-    <mergeCell ref="AW94:AX94"/>
     <mergeCell ref="AW95:AX95"/>
     <mergeCell ref="AW97:AX97"/>
     <mergeCell ref="AW98:AX98"/>
@@ -58939,6 +58939,8 @@
     <mergeCell ref="AW26:AY26"/>
     <mergeCell ref="AZ73:BA73"/>
     <mergeCell ref="AW90:AY90"/>
+    <mergeCell ref="BC86:BF86"/>
+    <mergeCell ref="AZ86:BA86"/>
     <mergeCell ref="AZ115:BA115"/>
     <mergeCell ref="BC115:BF115"/>
     <mergeCell ref="AZ109:BA109"/>
@@ -58971,8 +58973,6 @@
     <mergeCell ref="AW20:AY20"/>
     <mergeCell ref="AW21:AY21"/>
     <mergeCell ref="AW92:AY92"/>
-    <mergeCell ref="BC86:BF86"/>
-    <mergeCell ref="AZ86:BA86"/>
     <mergeCell ref="AZ87:BA87"/>
     <mergeCell ref="BC87:BF87"/>
     <mergeCell ref="BC93:BF93"/>
@@ -70398,13 +70398,13 @@
   <sheetData>
     <row r="3" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B3" s="231" t="s">
-        <v>3338</v>
+        <v>3333</v>
       </c>
       <c r="E3" s="231" t="s">
-        <v>3340</v>
+        <v>3335</v>
       </c>
       <c r="F3" s="231" t="s">
-        <v>3346</v>
+        <v>3341</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
@@ -70412,504 +70412,504 @@
         <v>1</v>
       </c>
       <c r="C4" s="232" t="s">
-        <v>3344</v>
+        <v>3339</v>
       </c>
       <c r="D4" s="232" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="232" t="s">
-        <v>3345</v>
+        <v>3340</v>
       </c>
       <c r="G4" s="232" t="s">
-        <v>3363</v>
+        <v>3358</v>
       </c>
       <c r="H4" s="232" t="s">
-        <v>3341</v>
+        <v>3336</v>
       </c>
       <c r="I4" s="232" t="s">
-        <v>3364</v>
+        <v>3359</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="102" x14ac:dyDescent="0.2">
       <c r="B5" s="231" t="s">
-        <v>3339</v>
+        <v>3334</v>
       </c>
       <c r="C5" s="231" t="s">
         <v>424</v>
       </c>
       <c r="D5" s="230" t="s">
-        <v>3361</v>
+        <v>3356</v>
       </c>
       <c r="E5" s="230" t="s">
-        <v>3370</v>
+        <v>3365</v>
       </c>
       <c r="F5" s="231" t="s">
-        <v>3347</v>
+        <v>3342</v>
       </c>
       <c r="G5" s="230" t="s">
-        <v>3362</v>
+        <v>3357</v>
       </c>
       <c r="H5" s="231" t="s">
-        <v>3342</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="231" t="s">
+        <v>3338</v>
+      </c>
+      <c r="C6" s="230" t="s">
         <v>3343</v>
-      </c>
-      <c r="C6" s="230" t="s">
-        <v>3348</v>
       </c>
       <c r="D6" s="230"/>
       <c r="E6" s="230" t="s">
-        <v>3350</v>
+        <v>3345</v>
       </c>
       <c r="F6" s="230" t="s">
-        <v>3351</v>
+        <v>3346</v>
       </c>
       <c r="G6" s="230"/>
     </row>
     <row r="7" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B7" s="230" t="s">
-        <v>3352</v>
+        <v>3347</v>
       </c>
       <c r="C7" s="230" t="s">
-        <v>3354</v>
+        <v>3349</v>
       </c>
       <c r="D7" s="230"/>
       <c r="E7" s="230" t="s">
-        <v>3359</v>
+        <v>3354</v>
       </c>
       <c r="G7" s="230"/>
       <c r="H7" s="230" t="s">
-        <v>3358</v>
+        <v>3353</v>
       </c>
       <c r="I7" s="230" t="s">
-        <v>3353</v>
+        <v>3348</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B8" s="230" t="s">
-        <v>3355</v>
+        <v>3350</v>
       </c>
       <c r="C8" s="230" t="s">
-        <v>3356</v>
+        <v>3351</v>
       </c>
       <c r="D8" s="230"/>
       <c r="E8" s="230" t="s">
-        <v>3357</v>
+        <v>3352</v>
       </c>
       <c r="G8" s="230"/>
       <c r="H8" s="230" t="s">
-        <v>3360</v>
+        <v>3355</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B9" s="230" t="s">
-        <v>3365</v>
+        <v>3360</v>
       </c>
       <c r="C9" s="230" t="s">
         <v>966</v>
       </c>
       <c r="D9" s="230" t="s">
-        <v>3366</v>
+        <v>3361</v>
       </c>
       <c r="E9" s="230" t="s">
-        <v>3369</v>
+        <v>3364</v>
       </c>
       <c r="G9" s="230" t="s">
-        <v>3367</v>
+        <v>3362</v>
       </c>
       <c r="I9" s="230" t="s">
-        <v>3368</v>
+        <v>3363</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B10" s="231" t="s">
-        <v>3371</v>
+        <v>3366</v>
       </c>
       <c r="C10" s="231" t="s">
-        <v>3372</v>
+        <v>3367</v>
       </c>
       <c r="D10" s="230" t="s">
-        <v>3373</v>
+        <v>3368</v>
       </c>
       <c r="E10" s="231" t="s">
-        <v>3374</v>
+        <v>3369</v>
       </c>
       <c r="G10" s="230" t="s">
-        <v>3384</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B11" s="231" t="s">
-        <v>3387</v>
+        <v>3382</v>
       </c>
       <c r="C11" s="231" t="s">
-        <v>3389</v>
+        <v>3384</v>
       </c>
       <c r="D11" s="231" t="s">
-        <v>3391</v>
+        <v>3386</v>
       </c>
       <c r="E11" s="231" t="s">
-        <v>3393</v>
+        <v>3388</v>
       </c>
       <c r="G11" s="231" t="s">
-        <v>3395</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B12" s="231" t="s">
-        <v>3388</v>
+        <v>3383</v>
       </c>
       <c r="C12" s="231" t="s">
+        <v>3385</v>
+      </c>
+      <c r="D12" s="231" t="s">
+        <v>3387</v>
+      </c>
+      <c r="E12" s="231" t="s">
+        <v>3389</v>
+      </c>
+      <c r="G12" s="231" t="s">
         <v>3390</v>
-      </c>
-      <c r="D12" s="231" t="s">
-        <v>3392</v>
-      </c>
-      <c r="E12" s="231" t="s">
-        <v>3394</v>
-      </c>
-      <c r="G12" s="231" t="s">
-        <v>3395</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="382.5" x14ac:dyDescent="0.2">
       <c r="B13" s="231" t="s">
-        <v>3401</v>
+        <v>3396</v>
       </c>
       <c r="C13" s="231" t="s">
-        <v>3402</v>
+        <v>3397</v>
       </c>
       <c r="D13" s="231" t="s">
-        <v>3403</v>
+        <v>3398</v>
       </c>
       <c r="E13" s="231" t="s">
-        <v>3404</v>
+        <v>3399</v>
       </c>
       <c r="F13" s="231" t="s">
-        <v>3349</v>
+        <v>3344</v>
       </c>
       <c r="G13" s="231" t="s">
-        <v>3402</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="382.5" x14ac:dyDescent="0.2">
       <c r="B14" s="231" t="s">
-        <v>3405</v>
+        <v>3400</v>
       </c>
       <c r="C14" s="231" t="s">
-        <v>3406</v>
+        <v>3401</v>
       </c>
       <c r="D14" s="231" t="s">
-        <v>3408</v>
+        <v>3403</v>
       </c>
       <c r="E14" s="231" t="s">
-        <v>3409</v>
+        <v>3404</v>
       </c>
       <c r="F14" s="231" t="s">
-        <v>3407</v>
+        <v>3402</v>
       </c>
       <c r="G14" s="231" t="s">
-        <v>3406</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="382.5" x14ac:dyDescent="0.2">
       <c r="B15" s="231" t="s">
-        <v>3405</v>
+        <v>3400</v>
       </c>
       <c r="C15" s="231" t="s">
-        <v>3411</v>
+        <v>3406</v>
       </c>
       <c r="D15" s="231" t="s">
-        <v>3408</v>
+        <v>3403</v>
       </c>
       <c r="E15" s="231" t="s">
-        <v>3409</v>
+        <v>3404</v>
       </c>
       <c r="F15" s="231" t="s">
-        <v>3407</v>
+        <v>3402</v>
       </c>
       <c r="G15" s="231" t="s">
-        <v>3406</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="382.5" x14ac:dyDescent="0.2">
       <c r="B16" s="231" t="s">
-        <v>3410</v>
+        <v>3405</v>
       </c>
       <c r="C16" s="231" t="s">
-        <v>3411</v>
+        <v>3406</v>
       </c>
       <c r="D16" s="231" t="s">
-        <v>3412</v>
+        <v>3407</v>
       </c>
       <c r="E16" s="231" t="s">
-        <v>3413</v>
+        <v>3408</v>
       </c>
       <c r="F16" s="231" t="s">
-        <v>3407</v>
+        <v>3402</v>
       </c>
       <c r="G16" s="231" t="s">
-        <v>3411</v>
+        <v>3406</v>
       </c>
     </row>
     <row r="17" spans="1:32" ht="369.75" x14ac:dyDescent="0.2">
       <c r="B17" s="231" t="s">
-        <v>3414</v>
+        <v>3409</v>
       </c>
       <c r="C17" s="231" t="s">
-        <v>3415</v>
+        <v>3410</v>
       </c>
       <c r="D17" s="231" t="s">
+        <v>3411</v>
+      </c>
+      <c r="E17" s="231" t="s">
         <v>3416</v>
       </c>
-      <c r="E17" s="231" t="s">
-        <v>3421</v>
-      </c>
       <c r="F17" s="231" t="s">
-        <v>3416</v>
+        <v>3411</v>
       </c>
       <c r="G17" s="231" t="s">
-        <v>3422</v>
+        <v>3417</v>
       </c>
       <c r="I17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="J17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="K17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="L17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="M17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="N17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="O17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="P17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="Q17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="R17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="S17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="T17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="U17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="V17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="W17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="X17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="Y17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="Z17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AA17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AB17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AC17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AD17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AE17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AF17" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="231" t="s">
-        <v>3418</v>
+        <v>3413</v>
       </c>
       <c r="B18" s="231" t="s">
-        <v>3419</v>
+        <v>3414</v>
       </c>
       <c r="C18" s="231" t="s">
         <v>960</v>
       </c>
       <c r="D18" s="231" t="s">
-        <v>3420</v>
+        <v>3415</v>
       </c>
       <c r="E18" s="231" t="s">
-        <v>3424</v>
+        <v>3419</v>
       </c>
       <c r="F18" s="231" t="s">
-        <v>3420</v>
+        <v>3415</v>
       </c>
       <c r="G18" s="231" t="s">
-        <v>3423</v>
+        <v>3418</v>
       </c>
       <c r="I18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="J18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="K18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="L18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="M18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="N18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="O18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="P18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="Q18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="R18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="S18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="T18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="U18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="V18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="W18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="X18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="Y18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="Z18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AA18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AB18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AC18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AD18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AE18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
       <c r="AF18" s="231" t="s">
-        <v>3417</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="102" x14ac:dyDescent="0.2">
       <c r="B19" s="231" t="s">
-        <v>3430</v>
+        <v>3425</v>
       </c>
       <c r="C19" s="231" t="s">
-        <v>3445</v>
+        <v>3440</v>
       </c>
       <c r="D19" s="231" t="s">
-        <v>3443</v>
+        <v>3438</v>
       </c>
       <c r="E19" s="231" t="s">
-        <v>3442</v>
+        <v>3437</v>
       </c>
       <c r="G19" s="230" t="s">
-        <v>3441</v>
+        <v>3436</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B20" s="231" t="s">
-        <v>3431</v>
+        <v>3426</v>
       </c>
       <c r="C20" s="231" t="s">
-        <v>3444</v>
+        <v>3439</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B21" s="231" t="s">
-        <v>3432</v>
+        <v>3427</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B22" s="231" t="s">
-        <v>3433</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B23" s="231" t="s">
-        <v>3434</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B24" s="231" t="s">
-        <v>3435</v>
+        <v>3430</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B25" s="231" t="s">
-        <v>3436</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B26" s="231" t="s">
-        <v>3437</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B27" s="231" t="s">
-        <v>3438</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B28" s="231" t="s">
-        <v>3439</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B29" s="231" t="s">
-        <v>3440</v>
+        <v>3435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>